<commit_message>
minor updates to errors
</commit_message>
<xml_diff>
--- a/data/reservingAccident/triangle.xlsx
+++ b/data/reservingAccident/triangle.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15950" windowHeight="6590" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15950" windowHeight="6590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="triangle" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="66">
   <si>
     <t>NA</t>
   </si>
@@ -29,9 +29,6 @@
     <t>Data as exported by R</t>
   </si>
   <si>
-    <t>Ultimate (vol weighted CL)</t>
-  </si>
-  <si>
     <t>Reserves</t>
   </si>
   <si>
@@ -192,19 +189,48 @@
   </si>
   <si>
     <t>25pct Tree</t>
+  </si>
+  <si>
+    <t>Inverse LDF</t>
+  </si>
+  <si>
+    <t>True Ultimate</t>
+  </si>
+  <si>
+    <t>True Reserve</t>
+  </si>
+  <si>
+    <t>Ultimate (volume weighted CL)</t>
+  </si>
+  <si>
+    <t>Age(months)–––––(1)</t>
+  </si>
+  <si>
+    <t>CumulativePaid Loss–––––(2)</t>
+  </si>
+  <si>
+    <t>SelectedDevelopmentFactors–––––(3)</t>
+  </si>
+  <si>
+    <t>CumulativeDevelopmentFactors–––––(4)</t>
+  </si>
+  <si>
+    <t>UltimateLoss(2) x (4)–––––(5)</t>
+  </si>
+  <si>
+    <t>12-24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0_;"/>
     <numFmt numFmtId="165" formatCode="#,##0.000_;"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000000000000_;"/>
     <numFmt numFmtId="167" formatCode="0.0000%"/>
     <numFmt numFmtId="168" formatCode="0.00000%"/>
-    <numFmt numFmtId="169" formatCode="#,##0.000000000000000000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -714,7 +740,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -736,8 +762,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1059,614 +1083,670 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI19"/>
+  <dimension ref="A1:AL19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="13" width="12.6328125" customWidth="1"/>
-    <col min="15" max="17" width="13.08984375" customWidth="1"/>
-    <col min="21" max="21" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="12.26953125" customWidth="1"/>
-    <col min="27" max="35" width="10.6328125" customWidth="1"/>
+    <col min="3" max="14" width="12.6328125" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="13.08984375" customWidth="1"/>
+    <col min="24" max="24" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="12.26953125" customWidth="1"/>
+    <col min="30" max="38" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B3">
+      <c r="AD1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>8</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>9</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>11</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>12</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="V3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="W3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>1994</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="C4" s="9">
         <v>54528825</v>
       </c>
-      <c r="C4" s="9">
+      <c r="D4" s="9">
         <v>84930173</v>
       </c>
-      <c r="D4" s="9">
+      <c r="E4" s="9">
         <v>95155175</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F4" s="9">
         <v>100076635</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G4" s="9">
         <v>102745306</v>
       </c>
-      <c r="G4" s="9">
+      <c r="H4" s="9">
         <v>104782943</v>
       </c>
-      <c r="H4" s="9">
+      <c r="I4" s="9">
         <v>106243585</v>
       </c>
-      <c r="I4" s="9">
+      <c r="J4" s="9">
         <v>107327580</v>
       </c>
-      <c r="J4" s="9">
+      <c r="K4" s="9">
         <v>108006131</v>
       </c>
-      <c r="K4" s="9">
+      <c r="L4" s="9">
         <v>108593649</v>
       </c>
-      <c r="L4" s="9">
+      <c r="M4" s="9">
         <v>109030127</v>
       </c>
-      <c r="M4" s="9">
+      <c r="N4" s="9">
         <v>109393653</v>
       </c>
-      <c r="O4" s="5">
-        <f>+AB4</f>
+      <c r="P4" s="5">
+        <f>+truth!A3</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>+T4+P4</f>
         <v>109393653</v>
       </c>
-      <c r="P4" s="5">
-        <f>+AH4</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <f>+AF4</f>
+      <c r="R4" s="5">
+        <f>+AE4</f>
         <v>109393653</v>
       </c>
-      <c r="R4" s="4">
-        <f t="shared" ref="R4:R15" si="0">+Q4/O4</f>
+      <c r="S4" s="5">
+        <f>+AK4</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <f>+AI4</f>
+        <v>109393653</v>
+      </c>
+      <c r="U4" s="4">
+        <f t="shared" ref="U4:U15" si="0">+T4/R4</f>
         <v>1</v>
       </c>
-      <c r="S4" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A4)</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="4"/>
-      <c r="U4" s="16">
-        <f ca="1">+OFFSET($M4,0,-A4+1)-Q4</f>
-        <v>0</v>
-      </c>
-      <c r="V4" s="15">
-        <f t="shared" ref="V4" si="1">+O4-P4-Q4</f>
-        <v>0</v>
-      </c>
-      <c r="W4" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A4)-R4</f>
-        <v>0</v>
-      </c>
-      <c r="X4" s="2">
-        <f t="shared" ref="X4:X14" si="2">+C4/$R$14</f>
+      <c r="V4" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B4)</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="4"/>
+      <c r="X4" s="16">
+        <f ca="1">+OFFSET($N4,0,-B4+1)-T4</f>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="15">
+        <f t="shared" ref="Y4" si="1">+R4-S4-T4</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B4)-U4</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2">
+        <f t="shared" ref="AA4:AA14" si="2">+D4/$U$14</f>
         <v>113174461.15040897</v>
       </c>
-      <c r="Y4" s="2">
-        <f t="shared" ref="Y4:Y14" si="3">+O4-X4</f>
+      <c r="AB4" s="2">
+        <f t="shared" ref="AB4:AB14" si="3">+R4-AA4</f>
         <v>-3780808.1504089683</v>
       </c>
-      <c r="AA4" s="7">
+      <c r="AD4" s="7">
         <v>34699</v>
-      </c>
-      <c r="AB4" s="8">
-        <v>109393653</v>
-      </c>
-      <c r="AC4" s="8">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="8">
-        <v>109393653</v>
       </c>
       <c r="AE4" s="8">
         <v>109393653</v>
       </c>
       <c r="AF4" s="8">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="8">
         <v>109393653</v>
       </c>
-      <c r="AG4" s="8">
-        <v>0</v>
-      </c>
       <c r="AH4" s="8">
-        <v>0</v>
+        <v>109393653</v>
       </c>
       <c r="AI4" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+        <v>109393653</v>
+      </c>
+      <c r="AJ4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f>1+A4</f>
+        <f>+A4+1</f>
+        <v>1995</v>
+      </c>
+      <c r="B5">
+        <f>1+B4</f>
         <v>2</v>
       </c>
-      <c r="B5" s="9">
+      <c r="C5" s="9">
         <v>52617643</v>
       </c>
-      <c r="C5" s="9">
+      <c r="D5" s="9">
         <v>82326081</v>
       </c>
-      <c r="D5" s="9">
+      <c r="E5" s="9">
         <v>92488762</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F5" s="9">
         <v>97083953</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="9">
         <v>99779085</v>
       </c>
-      <c r="G5" s="9">
+      <c r="H5" s="9">
         <v>101642338</v>
       </c>
-      <c r="H5" s="9">
+      <c r="I5" s="9">
         <v>103048081</v>
       </c>
-      <c r="I5" s="9">
+      <c r="J5" s="9">
         <v>104144626</v>
       </c>
-      <c r="J5" s="9">
+      <c r="K5" s="9">
         <v>104930498</v>
       </c>
-      <c r="K5" s="9">
+      <c r="L5" s="9">
         <v>105694105</v>
       </c>
-      <c r="L5" s="9">
+      <c r="M5" s="9">
         <v>106315346</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <f t="shared" ref="O5:O15" si="4">+AB5</f>
+      <c r="N5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
+        <f>+truth!A4</f>
+        <v>402632</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" ref="Q5:Q16" si="4">+T5+P5</f>
+        <v>106717978</v>
+      </c>
+      <c r="R5" s="5">
+        <f t="shared" ref="R5:R15" si="5">+AE5</f>
         <v>106669820.4332</v>
       </c>
-      <c r="P5" s="5">
-        <f t="shared" ref="P5:P15" si="5">+AH5</f>
+      <c r="S5" s="5">
+        <f t="shared" ref="S5:S15" si="6">+AK5</f>
         <v>354474.433199525</v>
       </c>
-      <c r="Q5" s="5">
-        <f t="shared" ref="Q5:Q15" si="6">+AF5</f>
+      <c r="T5" s="5">
+        <f t="shared" ref="T5:T15" si="7">+AI5</f>
         <v>106315346</v>
       </c>
-      <c r="R5" s="4">
+      <c r="U5" s="4">
         <f t="shared" si="0"/>
         <v>0.99667690044137658</v>
       </c>
-      <c r="S5" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A5)</f>
+      <c r="V5" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B5)</f>
         <v>1.0033341793686099</v>
       </c>
-      <c r="T5" s="4">
-        <f t="shared" ref="T5:T15" ca="1" si="7">1/S5</f>
+      <c r="W5" s="4">
+        <f t="shared" ref="W5:W15" ca="1" si="8">1/V5</f>
         <v>0.99667690044137824</v>
       </c>
-      <c r="U5" s="16">
-        <f t="shared" ref="U5:U15" ca="1" si="8">+OFFSET($M5,0,-A5+1)-Q5</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="15">
-        <f>+O5-P5-Q5</f>
+      <c r="X5" s="16">
+        <f t="shared" ref="X5:X15" ca="1" si="9">+OFFSET($N5,0,-B5+1)-T5</f>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="15">
+        <f>+R5-S5-T5</f>
         <v>4.76837158203125E-7</v>
       </c>
-      <c r="W5" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A5)-R5</f>
+      <c r="Z5" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B5)-U5</f>
         <v>4.4408920985006262E-15</v>
       </c>
-      <c r="X5" s="2">
+      <c r="AA5" s="2">
         <f t="shared" si="2"/>
         <v>109704355.08002464</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="AB5" s="2">
         <f t="shared" si="3"/>
         <v>-3034534.646824643</v>
       </c>
-      <c r="AA5" s="7">
+      <c r="AD5" s="7">
         <v>35064</v>
       </c>
-      <c r="AB5" s="8">
+      <c r="AE5" s="8">
         <v>106669820.4332</v>
       </c>
-      <c r="AC5" s="8">
+      <c r="AF5" s="8">
         <v>1</v>
       </c>
-      <c r="AD5" s="8">
+      <c r="AG5" s="8">
         <v>106669820.4332</v>
       </c>
-      <c r="AE5" s="8">
+      <c r="AH5" s="8">
         <v>106315346</v>
       </c>
-      <c r="AF5" s="8">
+      <c r="AI5" s="8">
         <v>106315346</v>
       </c>
-      <c r="AG5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="8">
+      <c r="AJ5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="8">
         <v>354474.433199525</v>
       </c>
-      <c r="AI5" s="8">
+      <c r="AL5" s="8">
         <v>354474.433199525</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" ref="A6:A15" si="9">1+A5</f>
+        <f t="shared" ref="A6:A15" si="10">+A5+1</f>
+        <v>1996</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B15" si="11">1+B5</f>
         <v>3</v>
       </c>
-      <c r="B6" s="9">
+      <c r="C6" s="9">
         <v>52802533</v>
       </c>
-      <c r="C6" s="9">
+      <c r="D6" s="9">
         <v>83811749</v>
       </c>
-      <c r="D6" s="9">
+      <c r="E6" s="9">
         <v>96639642</v>
       </c>
-      <c r="E6" s="9">
+      <c r="F6" s="9">
         <v>102574259</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
         <v>106289046</v>
       </c>
-      <c r="G6" s="9">
+      <c r="H6" s="9">
         <v>108676563</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="9">
         <v>110653125</v>
       </c>
-      <c r="I6" s="9">
+      <c r="J6" s="9">
         <v>111962351</v>
       </c>
-      <c r="J6" s="9">
+      <c r="K6" s="9">
         <v>112911041</v>
       </c>
-      <c r="K6" s="9">
+      <c r="L6" s="9">
         <v>113892219</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="M6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="5">
+      <c r="N6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <f>+truth!A5</f>
+        <v>1362840</v>
+      </c>
+      <c r="Q6" s="5">
         <f t="shared" si="4"/>
+        <v>115255059</v>
+      </c>
+      <c r="R6" s="5">
+        <f t="shared" si="5"/>
         <v>114835999.60712001</v>
       </c>
-      <c r="P6" s="5">
-        <f t="shared" si="5"/>
+      <c r="S6" s="5">
+        <f t="shared" si="6"/>
         <v>943780.60712005198</v>
       </c>
-      <c r="Q6" s="5">
-        <f t="shared" si="6"/>
+      <c r="T6" s="5">
+        <f t="shared" si="7"/>
         <v>113892219</v>
       </c>
-      <c r="R6" s="4">
+      <c r="U6" s="4">
         <f t="shared" si="0"/>
         <v>0.99178149177654307</v>
       </c>
-      <c r="S6" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A6)</f>
+      <c r="V6" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B6)</f>
         <v>1.0049359750161</v>
       </c>
-      <c r="T6" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W6" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.99508826916458937</v>
       </c>
-      <c r="U6" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="15">
-        <f t="shared" ref="V6:V15" si="10">+O6-P6-Q6</f>
-        <v>0</v>
-      </c>
-      <c r="W6" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A6)-R6</f>
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
+      <c r="X6" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="15">
+        <f t="shared" ref="Y6:Y15" si="12">+R6-S6-T6</f>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B6)-U6</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2">
         <f t="shared" si="2"/>
         <v>111684095.25255916</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="AB6" s="2">
         <f t="shared" si="3"/>
         <v>3151904.3545608521</v>
       </c>
-      <c r="AA6" s="7">
+      <c r="AD6" s="7">
         <v>35430</v>
       </c>
-      <c r="AB6" s="8">
+      <c r="AE6" s="8">
         <v>114835999.60712001</v>
       </c>
-      <c r="AC6" s="8">
+      <c r="AF6" s="8">
         <v>1</v>
       </c>
-      <c r="AD6" s="8">
+      <c r="AG6" s="8">
         <v>114835999.60712001</v>
       </c>
-      <c r="AE6" s="8">
+      <c r="AH6" s="8">
         <v>113892219</v>
       </c>
-      <c r="AF6" s="8">
+      <c r="AI6" s="8">
         <v>113892219</v>
       </c>
-      <c r="AG6" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="8">
+      <c r="AJ6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="8">
         <v>943780.60712005198</v>
       </c>
-      <c r="AI6" s="8">
+      <c r="AL6" s="8">
         <v>943780.60712005198</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>1997</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B7" s="9">
+      <c r="C7" s="9">
         <v>49838540</v>
       </c>
-      <c r="C7" s="9">
+      <c r="D7" s="9">
         <v>80421914</v>
       </c>
-      <c r="D7" s="9">
+      <c r="E7" s="9">
         <v>91873925</v>
       </c>
-      <c r="E7" s="9">
+      <c r="F7" s="9">
         <v>96987472</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
         <v>99474577</v>
       </c>
-      <c r="G7" s="9">
+      <c r="H7" s="9">
         <v>101271088</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
         <v>102774844</v>
       </c>
-      <c r="I7" s="9">
+      <c r="J7" s="9">
         <v>103992270</v>
       </c>
-      <c r="J7" s="9">
+      <c r="K7" s="9">
         <v>105035099</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="L7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O7" s="5">
+      <c r="N7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <f>+truth!A6</f>
+        <v>2052225</v>
+      </c>
+      <c r="Q7" s="5">
         <f t="shared" si="4"/>
+        <v>107087324</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" si="5"/>
         <v>106663518.29318801</v>
       </c>
-      <c r="P7" s="5">
-        <f t="shared" si="5"/>
+      <c r="S7" s="5">
+        <f t="shared" si="6"/>
         <v>1628419.29318833</v>
       </c>
-      <c r="Q7" s="5">
-        <f t="shared" si="6"/>
+      <c r="T7" s="5">
+        <f t="shared" si="7"/>
         <v>105035099</v>
       </c>
-      <c r="R7" s="4">
+      <c r="U7" s="4">
         <f t="shared" si="0"/>
         <v>0.98473311850906753</v>
       </c>
-      <c r="S7" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A7)</f>
+      <c r="V7" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B7)</f>
         <v>1.0071576482348299</v>
       </c>
-      <c r="T7" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W7" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.99289321959936006</v>
       </c>
-      <c r="U7" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="15">
-        <f t="shared" si="10"/>
+      <c r="X7" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="15">
+        <f t="shared" si="12"/>
         <v>-3.2782554626464844E-7</v>
       </c>
-      <c r="W7" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A7)-R7</f>
+      <c r="Z7" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B7)-U7</f>
         <v>-2.55351295663786E-15</v>
       </c>
-      <c r="X7" s="2">
+      <c r="AA7" s="2">
         <f t="shared" si="2"/>
         <v>107166940.32443018</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="AB7" s="2">
         <f t="shared" si="3"/>
         <v>-503422.03124217689</v>
       </c>
-      <c r="AA7" s="7">
+      <c r="AD7" s="7">
         <v>35795</v>
       </c>
-      <c r="AB7" s="8">
+      <c r="AE7" s="8">
         <v>106663518.29318801</v>
       </c>
-      <c r="AC7" s="8">
+      <c r="AF7" s="8">
         <v>1</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AG7" s="8">
         <v>106663518.29318801</v>
       </c>
-      <c r="AE7" s="8">
+      <c r="AH7" s="8">
         <v>105035099</v>
       </c>
-      <c r="AF7" s="8">
+      <c r="AI7" s="8">
         <v>105035099</v>
       </c>
-      <c r="AG7" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="8">
+      <c r="AJ7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="8">
         <v>1628419.29318833</v>
       </c>
-      <c r="AI7" s="8">
+      <c r="AL7" s="8">
         <v>1628419.29318833</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>1998</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="B8" s="9">
+      <c r="C8" s="9">
         <v>52703836</v>
       </c>
-      <c r="C8" s="9">
+      <c r="D8" s="9">
         <v>86610906</v>
       </c>
-      <c r="D8" s="9">
+      <c r="E8" s="9">
         <v>97974767</v>
       </c>
-      <c r="E8" s="9">
+      <c r="F8" s="9">
         <v>103425365</v>
       </c>
-      <c r="F8" s="9">
+      <c r="G8" s="9">
         <v>106515923</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="9">
         <v>108683986</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9">
         <v>110216385</v>
       </c>
-      <c r="I8" s="9">
+      <c r="J8" s="9">
         <v>111470947</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="K8" s="9" t="s">
         <v>0</v>
       </c>
@@ -1676,107 +1756,119 @@
       <c r="M8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="5">
+      <c r="N8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
+        <f>+truth!A7</f>
+        <v>2932050</v>
+      </c>
+      <c r="Q8" s="5">
         <f t="shared" si="4"/>
+        <v>114402997</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="5"/>
         <v>114114411.953134</v>
       </c>
-      <c r="P8" s="5">
-        <f t="shared" si="5"/>
+      <c r="S8" s="5">
+        <f t="shared" si="6"/>
         <v>2643464.9531339598</v>
       </c>
-      <c r="Q8" s="5">
-        <f t="shared" si="6"/>
+      <c r="T8" s="5">
+        <f t="shared" si="7"/>
         <v>111470947</v>
       </c>
-      <c r="R8" s="4">
+      <c r="U8" s="4">
         <f t="shared" si="0"/>
         <v>0.9768349596874788</v>
       </c>
-      <c r="S8" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A8)</f>
+      <c r="V8" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B8)</f>
         <v>1.00808545880065</v>
       </c>
-      <c r="T8" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W8" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.99197939149894143</v>
       </c>
-      <c r="U8" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V8" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A8)-R8</f>
-        <v>0</v>
-      </c>
-      <c r="X8" s="2">
+      <c r="X8" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B8)-U8</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2">
         <f t="shared" si="2"/>
         <v>115414136.93221517</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="AB8" s="2">
         <f t="shared" si="3"/>
         <v>-1299724.9790811688</v>
       </c>
-      <c r="AA8" s="7">
+      <c r="AD8" s="7">
         <v>36160</v>
       </c>
-      <c r="AB8" s="8">
+      <c r="AE8" s="8">
         <v>114114411.953134</v>
       </c>
-      <c r="AC8" s="8">
+      <c r="AF8" s="8">
         <v>1</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AG8" s="8">
         <v>114114411.953134</v>
       </c>
-      <c r="AE8" s="8">
+      <c r="AH8" s="8">
         <v>111470947</v>
       </c>
-      <c r="AF8" s="8">
+      <c r="AI8" s="8">
         <v>111470947</v>
       </c>
-      <c r="AG8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="8">
+      <c r="AJ8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="8">
         <v>2643464.9531339598</v>
       </c>
-      <c r="AI8" s="8">
+      <c r="AL8" s="8">
         <v>2643464.9531339598</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>1999</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="B9" s="9">
+      <c r="C9" s="9">
         <v>53858548</v>
       </c>
-      <c r="C9" s="9">
+      <c r="D9" s="9">
         <v>89297134</v>
       </c>
-      <c r="D9" s="9">
+      <c r="E9" s="9">
         <v>103023703</v>
       </c>
-      <c r="E9" s="9">
+      <c r="F9" s="9">
         <v>109080056</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="9">
         <v>112420272</v>
       </c>
-      <c r="G9" s="9">
+      <c r="H9" s="9">
         <v>114531877</v>
       </c>
-      <c r="H9" s="9">
+      <c r="I9" s="9">
         <v>115966335</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="J9" s="9" t="s">
         <v>0</v>
       </c>
@@ -1789,104 +1881,116 @@
       <c r="M9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="5">
+      <c r="N9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
+        <f>+truth!A8</f>
+        <v>3760055</v>
+      </c>
+      <c r="Q9" s="5">
         <f t="shared" si="4"/>
+        <v>119726390</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="5"/>
         <v>120044440.909565</v>
       </c>
-      <c r="P9" s="5">
-        <f t="shared" si="5"/>
+      <c r="S9" s="5">
+        <f t="shared" si="6"/>
         <v>4078105.90956512</v>
       </c>
-      <c r="Q9" s="5">
-        <f t="shared" si="6"/>
+      <c r="T9" s="5">
+        <f t="shared" si="7"/>
         <v>115966335</v>
       </c>
-      <c r="R9" s="4">
+      <c r="U9" s="4">
         <f t="shared" si="0"/>
         <v>0.96602836517321755</v>
       </c>
-      <c r="S9" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A9)</f>
+      <c r="V9" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B9)</f>
         <v>1.0111866223641599</v>
       </c>
-      <c r="T9" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W9" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.98893713374292325</v>
       </c>
-      <c r="U9" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V9" s="15">
-        <f t="shared" si="10"/>
+      <c r="X9" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="15">
+        <f t="shared" si="12"/>
         <v>-1.1920928955078125E-7</v>
       </c>
-      <c r="W9" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A9)-R9</f>
-        <v>0</v>
-      </c>
-      <c r="X9" s="2">
+      <c r="Z9" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B9)-U9</f>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
         <f t="shared" si="2"/>
         <v>118993694.06354399</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="AB9" s="2">
         <f t="shared" si="3"/>
         <v>1050746.8460210115</v>
       </c>
-      <c r="AA9" s="7">
+      <c r="AD9" s="7">
         <v>36525</v>
       </c>
-      <c r="AB9" s="8">
+      <c r="AE9" s="8">
         <v>120044440.909565</v>
       </c>
-      <c r="AC9" s="8">
+      <c r="AF9" s="8">
         <v>1</v>
       </c>
-      <c r="AD9" s="8">
+      <c r="AG9" s="8">
         <v>120044440.909565</v>
       </c>
-      <c r="AE9" s="8">
+      <c r="AH9" s="8">
         <v>115966335</v>
       </c>
-      <c r="AF9" s="8">
+      <c r="AI9" s="8">
         <v>115966335</v>
       </c>
-      <c r="AG9" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="8">
+      <c r="AJ9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="8">
         <v>4078105.90956512</v>
       </c>
-      <c r="AI9" s="8">
+      <c r="AL9" s="8">
         <v>4078105.90956512</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>2000</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="B10" s="9">
+      <c r="C10" s="9">
         <v>54694527</v>
       </c>
-      <c r="C10" s="9">
+      <c r="D10" s="9">
         <v>90220052</v>
       </c>
-      <c r="D10" s="9">
+      <c r="E10" s="9">
         <v>102634248</v>
       </c>
-      <c r="E10" s="9">
+      <c r="F10" s="9">
         <v>108224574</v>
       </c>
-      <c r="F10" s="9">
+      <c r="G10" s="9">
         <v>111341566</v>
       </c>
-      <c r="G10" s="9">
+      <c r="H10" s="9">
         <v>113418617</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="I10" s="9" t="s">
         <v>0</v>
       </c>
@@ -1902,101 +2006,113 @@
       <c r="M10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="5">
+      <c r="N10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <f>+truth!A9</f>
+        <v>5584206</v>
+      </c>
+      <c r="Q10" s="5">
         <f t="shared" si="4"/>
+        <v>119002823</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="5"/>
         <v>119116787.493789</v>
       </c>
-      <c r="P10" s="5">
-        <f t="shared" si="5"/>
+      <c r="S10" s="5">
+        <f t="shared" si="6"/>
         <v>5698170.4937885301</v>
       </c>
-      <c r="Q10" s="5">
-        <f t="shared" si="6"/>
+      <c r="T10" s="5">
+        <f t="shared" si="7"/>
         <v>113418617</v>
       </c>
-      <c r="R10" s="4">
+      <c r="U10" s="4">
         <f t="shared" si="0"/>
         <v>0.95216316177024063</v>
       </c>
-      <c r="S10" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A10)</f>
+      <c r="V10" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B10)</f>
         <v>1.01456179356613</v>
       </c>
-      <c r="T10" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W10" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.9856472088161865</v>
       </c>
-      <c r="U10" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V10" s="15">
-        <f t="shared" si="10"/>
+      <c r="X10" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="15">
+        <f t="shared" si="12"/>
         <v>4.76837158203125E-7</v>
       </c>
-      <c r="W10" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A10)-R10</f>
+      <c r="Z10" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B10)-U10</f>
         <v>4.3298697960381105E-15</v>
       </c>
-      <c r="X10" s="2">
+      <c r="AA10" s="2">
         <f t="shared" si="2"/>
         <v>120223536.69363038</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="AB10" s="2">
         <f t="shared" si="3"/>
         <v>-1106749.1998413801</v>
       </c>
-      <c r="AA10" s="7">
+      <c r="AD10" s="7">
         <v>36891</v>
       </c>
-      <c r="AB10" s="8">
+      <c r="AE10" s="8">
         <v>119116787.493789</v>
       </c>
-      <c r="AC10" s="8">
+      <c r="AF10" s="8">
         <v>1</v>
       </c>
-      <c r="AD10" s="8">
+      <c r="AG10" s="8">
         <v>119116787.493789</v>
       </c>
-      <c r="AE10" s="8">
+      <c r="AH10" s="8">
         <v>113418617</v>
       </c>
-      <c r="AF10" s="8">
+      <c r="AI10" s="8">
         <v>113418617</v>
       </c>
-      <c r="AG10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="8">
+      <c r="AJ10" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="8">
         <v>5698170.4937885301</v>
       </c>
-      <c r="AI10" s="8">
+      <c r="AL10" s="8">
         <v>5698170.4937885301</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>2001</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="B11" s="9">
+      <c r="C11" s="9">
         <v>58603881</v>
       </c>
-      <c r="C11" s="9">
+      <c r="D11" s="9">
         <v>96002420</v>
       </c>
-      <c r="D11" s="9">
+      <c r="E11" s="9">
         <v>110246744</v>
       </c>
-      <c r="E11" s="9">
+      <c r="F11" s="9">
         <v>116594418</v>
       </c>
-      <c r="F11" s="9">
+      <c r="G11" s="9">
         <v>120298776</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="H11" s="9" t="s">
         <v>0</v>
       </c>
@@ -2015,98 +2131,110 @@
       <c r="M11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O11" s="5">
+      <c r="N11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <f>+truth!A10</f>
+        <v>7233582</v>
+      </c>
+      <c r="Q11" s="5">
         <f t="shared" si="4"/>
+        <v>127532358</v>
+      </c>
+      <c r="R11" s="5">
+        <f t="shared" si="5"/>
         <v>128813062.5953</v>
       </c>
-      <c r="P11" s="5">
-        <f t="shared" si="5"/>
+      <c r="S11" s="5">
+        <f t="shared" si="6"/>
         <v>8514286.5953000207</v>
       </c>
-      <c r="Q11" s="5">
-        <f t="shared" si="6"/>
+      <c r="T11" s="5">
+        <f t="shared" si="7"/>
         <v>120298776</v>
       </c>
-      <c r="R11" s="4">
+      <c r="U11" s="4">
         <f t="shared" si="0"/>
         <v>0.93390199391462447</v>
       </c>
-      <c r="S11" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A11)</f>
+      <c r="V11" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B11)</f>
         <v>1.01955362337227</v>
       </c>
-      <c r="T11" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W11" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.98082138798389584</v>
       </c>
-      <c r="U11" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V11" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="W11" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A11)-R11</f>
-        <v>0</v>
-      </c>
-      <c r="X11" s="2">
+      <c r="X11" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B11)-U11</f>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
         <f t="shared" si="2"/>
         <v>127928882.85574603</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="AB11" s="2">
         <f t="shared" si="3"/>
         <v>884179.73955397308</v>
       </c>
-      <c r="AA11" s="7">
+      <c r="AD11" s="7">
         <v>37256</v>
       </c>
-      <c r="AB11" s="8">
+      <c r="AE11" s="8">
         <v>128813062.5953</v>
       </c>
-      <c r="AC11" s="8">
+      <c r="AF11" s="8">
         <v>1</v>
       </c>
-      <c r="AD11" s="8">
+      <c r="AG11" s="8">
         <v>128813062.5953</v>
       </c>
-      <c r="AE11" s="8">
+      <c r="AH11" s="8">
         <v>120298776</v>
       </c>
-      <c r="AF11" s="8">
+      <c r="AI11" s="8">
         <v>120298776</v>
       </c>
-      <c r="AG11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="8">
+      <c r="AJ11" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="8">
         <v>8514286.5953000207</v>
       </c>
-      <c r="AI11" s="8">
+      <c r="AL11" s="8">
         <v>8514286.5953000207</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>2002</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="B12" s="9">
+      <c r="C12" s="9">
         <v>56264364</v>
       </c>
-      <c r="C12" s="9">
+      <c r="D12" s="9">
         <v>91765553</v>
       </c>
-      <c r="D12" s="9">
+      <c r="E12" s="9">
         <v>105111550</v>
       </c>
-      <c r="E12" s="9">
+      <c r="F12" s="9">
         <v>111774418</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="G12" s="9" t="s">
         <v>0</v>
       </c>
@@ -2128,95 +2256,107 @@
       <c r="M12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O12" s="5">
+      <c r="N12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
+        <f>+truth!A11</f>
+        <v>12818962</v>
+      </c>
+      <c r="Q12" s="5">
         <f t="shared" si="4"/>
+        <v>124593380</v>
+      </c>
+      <c r="R12" s="5">
+        <f t="shared" si="5"/>
         <v>123246730.605801</v>
       </c>
-      <c r="P12" s="5">
-        <f t="shared" si="5"/>
+      <c r="S12" s="5">
+        <f t="shared" si="6"/>
         <v>11472312.6058012</v>
       </c>
-      <c r="Q12" s="5">
-        <f t="shared" si="6"/>
+      <c r="T12" s="5">
+        <f t="shared" si="7"/>
         <v>111774418</v>
       </c>
-      <c r="R12" s="4">
+      <c r="U12" s="4">
         <f t="shared" si="0"/>
         <v>0.90691588694149894</v>
       </c>
-      <c r="S12" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A12)</f>
+      <c r="V12" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B12)</f>
         <v>1.0297559094086799</v>
       </c>
-      <c r="T12" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W12" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.97110391973786614</v>
       </c>
-      <c r="U12" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V12" s="15">
-        <f t="shared" si="10"/>
+      <c r="X12" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="15">
+        <f t="shared" si="12"/>
         <v>-1.9371509552001953E-7</v>
       </c>
-      <c r="W12" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A12)-R12</f>
+      <c r="Z12" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B12)-U12</f>
         <v>-8.8817841970012523E-16</v>
       </c>
-      <c r="X12" s="2">
+      <c r="AA12" s="2">
         <f t="shared" si="2"/>
         <v>122283007.86511168</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="AB12" s="2">
         <f t="shared" si="3"/>
         <v>963722.74068932235</v>
       </c>
-      <c r="AA12" s="7">
+      <c r="AD12" s="7">
         <v>37621</v>
       </c>
-      <c r="AB12" s="8">
+      <c r="AE12" s="8">
         <v>123246730.605801</v>
       </c>
-      <c r="AC12" s="8">
+      <c r="AF12" s="8">
         <v>1</v>
       </c>
-      <c r="AD12" s="8">
+      <c r="AG12" s="8">
         <v>123246730.605801</v>
       </c>
-      <c r="AE12" s="8">
+      <c r="AH12" s="8">
         <v>111774418</v>
       </c>
-      <c r="AF12" s="8">
+      <c r="AI12" s="8">
         <v>111774418</v>
       </c>
-      <c r="AG12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="8">
+      <c r="AJ12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="8">
         <v>11472312.6058012</v>
       </c>
-      <c r="AI12" s="8">
+      <c r="AL12" s="8">
         <v>11472312.6058012</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>2003</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="B13" s="9">
+      <c r="C13" s="9">
         <v>65821493</v>
       </c>
-      <c r="C13" s="9">
+      <c r="D13" s="9">
         <v>111321226</v>
       </c>
-      <c r="D13" s="9">
+      <c r="E13" s="9">
         <v>130480200</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="F13" s="9" t="s">
         <v>0</v>
       </c>
@@ -2241,92 +2381,104 @@
       <c r="M13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="5">
+      <c r="N13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" s="5">
+        <f>+truth!A12</f>
+        <v>24357870</v>
+      </c>
+      <c r="Q13" s="5">
         <f t="shared" si="4"/>
+        <v>154838070</v>
+      </c>
+      <c r="R13" s="5">
+        <f t="shared" si="5"/>
         <v>152016780.03952101</v>
       </c>
-      <c r="P13" s="5">
-        <f t="shared" si="5"/>
+      <c r="S13" s="5">
+        <f t="shared" si="6"/>
         <v>21536580.039520599</v>
       </c>
-      <c r="Q13" s="5">
-        <f t="shared" si="6"/>
+      <c r="T13" s="5">
+        <f t="shared" si="7"/>
         <v>130480200</v>
       </c>
-      <c r="R13" s="4">
+      <c r="U13" s="4">
         <f t="shared" si="0"/>
         <v>0.85832761334688201</v>
       </c>
-      <c r="S13" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A13)</f>
+      <c r="V13" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B13)</f>
         <v>1.0566080746314901</v>
       </c>
-      <c r="T13" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W13" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.94642471888052426</v>
       </c>
-      <c r="U13" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="15">
-        <f t="shared" si="10"/>
+      <c r="X13" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="15">
+        <f t="shared" si="12"/>
         <v>4.1723251342773438E-7</v>
       </c>
-      <c r="W13" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A13)-R13</f>
+      <c r="Z13" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B13)-U13</f>
         <v>1.9984014443252818E-15</v>
       </c>
-      <c r="X13" s="2">
+      <c r="AA13" s="2">
         <f t="shared" si="2"/>
         <v>148342094.71294609</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="AB13" s="2">
         <f t="shared" si="3"/>
         <v>3674685.3265749216</v>
       </c>
-      <c r="AA13" s="7">
+      <c r="AD13" s="7">
         <v>37986</v>
       </c>
-      <c r="AB13" s="8">
+      <c r="AE13" s="8">
         <v>152016780.03952101</v>
       </c>
-      <c r="AC13" s="8">
+      <c r="AF13" s="8">
         <v>1</v>
       </c>
-      <c r="AD13" s="8">
+      <c r="AG13" s="8">
         <v>152016780.03952101</v>
       </c>
-      <c r="AE13" s="8">
+      <c r="AH13" s="8">
         <v>130480200</v>
       </c>
-      <c r="AF13" s="8">
+      <c r="AI13" s="8">
         <v>130480200</v>
       </c>
-      <c r="AG13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="8">
+      <c r="AJ13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="8">
         <v>21536580.039520599</v>
       </c>
-      <c r="AI13" s="8">
+      <c r="AL13" s="8">
         <v>21536580.039520599</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>2004</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="B14" s="9">
+      <c r="C14" s="9">
         <v>62052422</v>
       </c>
-      <c r="C14" s="9">
+      <c r="D14" s="9">
         <v>100442115</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="E14" s="9" t="s">
         <v>0</v>
       </c>
@@ -2354,89 +2506,101 @@
       <c r="M14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O14" s="5">
+      <c r="N14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
+        <f>+truth!A13</f>
+        <v>31901613</v>
+      </c>
+      <c r="Q14" s="5">
         <f t="shared" si="4"/>
+        <v>132343728</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" si="5"/>
         <v>133845038.110689</v>
       </c>
-      <c r="P14" s="5">
-        <f t="shared" si="5"/>
+      <c r="S14" s="5">
+        <f t="shared" si="6"/>
         <v>33402923.1106891</v>
       </c>
-      <c r="Q14" s="5">
-        <f t="shared" si="6"/>
+      <c r="T14" s="5">
+        <f t="shared" si="7"/>
         <v>100442115</v>
       </c>
-      <c r="R14" s="4">
+      <c r="U14" s="4">
         <f t="shared" si="0"/>
         <v>0.7504358504267824</v>
       </c>
-      <c r="S14" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A14)</f>
+      <c r="V14" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B14)</f>
         <v>1.1437721330327499</v>
       </c>
-      <c r="T14" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W14" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.87430002106142124</v>
       </c>
-      <c r="U14" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="W14" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A14)-R14</f>
-        <v>0</v>
-      </c>
-      <c r="X14" s="2">
+      <c r="X14" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B14)-U14</f>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
         <f t="shared" si="2"/>
         <v>133845038.110689</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="AB14" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="7">
+      <c r="AD14" s="7">
         <v>38352</v>
       </c>
-      <c r="AB14" s="8">
+      <c r="AE14" s="8">
         <v>133845038.110689</v>
       </c>
-      <c r="AC14" s="8">
+      <c r="AF14" s="8">
         <v>1</v>
       </c>
-      <c r="AD14" s="8">
+      <c r="AG14" s="8">
         <v>133845038.110689</v>
       </c>
-      <c r="AE14" s="8">
+      <c r="AH14" s="8">
         <v>100442115</v>
       </c>
-      <c r="AF14" s="8">
+      <c r="AI14" s="8">
         <v>100442115</v>
       </c>
-      <c r="AG14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="8">
+      <c r="AJ14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="8">
         <v>33402923.1106891</v>
       </c>
-      <c r="AI14" s="8">
+      <c r="AL14" s="8">
         <v>33402923.1106891</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>2005</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="B15" s="9">
+      <c r="C15" s="9">
         <v>68388763</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="D15" s="9" t="s">
         <v>0</v>
       </c>
@@ -2467,128 +2631,147 @@
       <c r="M15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O15" s="5">
+      <c r="N15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <f>+truth!A14</f>
+        <v>77968325</v>
+      </c>
+      <c r="Q15" s="5">
         <f t="shared" si="4"/>
+        <v>146357088</v>
+      </c>
+      <c r="R15" s="5">
+        <f t="shared" si="5"/>
         <v>148051892.25139701</v>
       </c>
-      <c r="P15" s="5">
-        <f t="shared" si="5"/>
+      <c r="S15" s="5">
+        <f t="shared" si="6"/>
         <v>79663129.251397505</v>
       </c>
-      <c r="Q15" s="5">
-        <f t="shared" si="6"/>
+      <c r="T15" s="5">
+        <f t="shared" si="7"/>
         <v>68388763</v>
       </c>
-      <c r="R15" s="4">
+      <c r="U15" s="4">
         <f t="shared" si="0"/>
         <v>0.46192427506345962</v>
       </c>
-      <c r="S15" s="4">
-        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-A15)</f>
+      <c r="V15" s="4">
+        <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B15)</f>
         <v>1.6245863032932999</v>
       </c>
-      <c r="T15" s="4">
-        <f t="shared" ca="1" si="7"/>
+      <c r="W15" s="4">
+        <f t="shared" ca="1" si="8"/>
         <v>0.61554132148771523</v>
       </c>
-      <c r="U15" s="16">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V15" s="15">
-        <f t="shared" si="10"/>
+      <c r="X15" s="16">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="15">
+        <f t="shared" si="12"/>
         <v>-4.9173831939697266E-7</v>
       </c>
-      <c r="W15" s="16">
-        <f ca="1">+OFFSET(LDFs!$A$26,0,13-A15)-R15</f>
+      <c r="Z15" s="16">
+        <f ca="1">+OFFSET(LDFs!$A$26,0,13-B15)-U15</f>
         <v>-1.609823385706477E-15</v>
       </c>
-      <c r="X15" s="2"/>
-      <c r="AA15" s="7">
+      <c r="AA15" s="2"/>
+      <c r="AD15" s="7">
         <v>38717</v>
       </c>
-      <c r="AB15" s="8">
+      <c r="AE15" s="8">
         <v>148051892.25139701</v>
       </c>
-      <c r="AC15" s="8">
+      <c r="AF15" s="8">
         <v>1</v>
       </c>
-      <c r="AD15" s="8">
+      <c r="AG15" s="8">
         <v>148051892.25139701</v>
       </c>
-      <c r="AE15" s="8">
+      <c r="AH15" s="8">
         <v>68388763</v>
       </c>
-      <c r="AF15" s="8">
+      <c r="AI15" s="8">
         <v>68388763</v>
       </c>
-      <c r="AG15" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="8">
+      <c r="AJ15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="8">
         <v>79663129.251397505</v>
       </c>
-      <c r="AI15" s="8">
+      <c r="AL15" s="8">
         <v>79663129.251397505</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="O16" s="6">
-        <f>+SUM(O4:O15)</f>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="P16" s="6">
+        <f>+truth!A15</f>
+        <v>170374360</v>
+      </c>
+      <c r="Q16" s="6">
+        <f t="shared" si="4"/>
+        <v>1477250848</v>
+      </c>
+      <c r="R16" s="6">
+        <f>+SUM(R4:R15)</f>
         <v>1476812135.2927041</v>
       </c>
-      <c r="P16" s="6">
-        <f>+SUM(P4:P15)</f>
+      <c r="S16" s="6">
+        <f>+SUM(S4:S15)</f>
         <v>169935647.29270393</v>
       </c>
-      <c r="Q16" s="6">
-        <f>+SUM(Q4:Q15)</f>
+      <c r="T16" s="6">
+        <f>+SUM(T4:T15)</f>
         <v>1306876488</v>
       </c>
-      <c r="U16" s="16">
-        <f ca="1">+SUM(U4:U15)</f>
-        <v>0</v>
-      </c>
-      <c r="V16" s="15">
-        <f>+SUM(V4:V15)</f>
+      <c r="X16" s="16">
+        <f ca="1">+SUM(X4:X15)</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="15">
+        <f>+SUM(Y4:Y15)</f>
         <v>2.384185791015625E-7</v>
       </c>
-      <c r="W16" s="16">
-        <f ca="1">+SUM(W4:W15)</f>
+      <c r="Z16" s="16">
+        <f ca="1">+SUM(Z4:Z15)</f>
         <v>5.7176485768195562E-15</v>
       </c>
-      <c r="AA16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB16" s="8">
+      <c r="AD16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE16" s="8">
         <v>1476812135.2927001</v>
       </c>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8">
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8">
         <v>1476812135.2927001</v>
       </c>
-      <c r="AE16" s="8">
+      <c r="AH16" s="8">
         <v>1306876488</v>
       </c>
-      <c r="AF16" s="8">
+      <c r="AI16" s="8">
         <v>1306876488</v>
       </c>
-      <c r="AG16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="8">
+      <c r="AJ16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="8">
         <v>169935647.29270399</v>
       </c>
-      <c r="AI16" s="8">
+      <c r="AL16" s="8">
         <v>169935647.29270399</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="O18" s="17"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="O19" s="18"/>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="R19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2598,58 +2781,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" customWidth="1"/>
+    <col min="18" max="18" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="11">
-        <v>45627</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>34699</v>
       </c>
@@ -2686,8 +2890,26 @@
       <c r="L2">
         <v>1.0033341793686099</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P2" s="10">
+        <v>34699</v>
+      </c>
+      <c r="Q2">
+        <v>144</v>
+      </c>
+      <c r="R2" s="2">
+        <v>109393653</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="2">
+        <v>109393653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>35064</v>
       </c>
@@ -2721,8 +2943,26 @@
       <c r="K3">
         <v>1.0058777261040199</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P3" s="10">
+        <v>35064</v>
+      </c>
+      <c r="Q3">
+        <v>132</v>
+      </c>
+      <c r="R3" s="2">
+        <v>106315346</v>
+      </c>
+      <c r="S3">
+        <v>1.0033341793686099</v>
+      </c>
+      <c r="T3">
+        <v>1.0033341793686099</v>
+      </c>
+      <c r="U3" s="2">
+        <v>106669820.4332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>35430</v>
       </c>
@@ -2753,8 +2993,26 @@
       <c r="J4">
         <v>1.00868983220162</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P4" s="10">
+        <v>35430</v>
+      </c>
+      <c r="Q4">
+        <v>120</v>
+      </c>
+      <c r="R4" s="2">
+        <v>113892219</v>
+      </c>
+      <c r="S4">
+        <v>1.0049359750161</v>
+      </c>
+      <c r="T4">
+        <v>1.0082866118107701</v>
+      </c>
+      <c r="U4" s="2">
+        <v>114835999.60712001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>35795</v>
       </c>
@@ -2782,8 +3040,26 @@
       <c r="I5">
         <v>1.0100279472695399</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P5" s="10">
+        <v>35795</v>
+      </c>
+      <c r="Q5">
+        <v>108</v>
+      </c>
+      <c r="R5" s="2">
+        <v>105035099</v>
+      </c>
+      <c r="S5">
+        <v>1.0071576482348299</v>
+      </c>
+      <c r="T5">
+        <v>1.015503572698</v>
+      </c>
+      <c r="U5" s="2">
+        <v>106663518.29318801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>36160</v>
       </c>
@@ -2808,8 +3084,26 @@
       <c r="H6">
         <v>1.01138271773294</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P6" s="10">
+        <v>36160</v>
+      </c>
+      <c r="Q6">
+        <v>96</v>
+      </c>
+      <c r="R6" s="2">
+        <v>111470947</v>
+      </c>
+      <c r="S6">
+        <v>1.00808545880065</v>
+      </c>
+      <c r="T6">
+        <v>1.0237143849969601</v>
+      </c>
+      <c r="U6" s="2">
+        <v>114114411.953134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>36525</v>
       </c>
@@ -2831,8 +3125,26 @@
       <c r="G7">
         <v>1.01252453061605</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P7" s="10">
+        <v>36525</v>
+      </c>
+      <c r="Q7">
+        <v>84</v>
+      </c>
+      <c r="R7" s="2">
+        <v>115966335</v>
+      </c>
+      <c r="S7">
+        <v>1.0111866223641599</v>
+      </c>
+      <c r="T7">
+        <v>1.03516629123068</v>
+      </c>
+      <c r="U7" s="2">
+        <v>120044440.909565</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>36891</v>
       </c>
@@ -2851,8 +3163,26 @@
       <c r="F8">
         <v>1.0186547672591599</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P8" s="10">
+        <v>36891</v>
+      </c>
+      <c r="Q8">
+        <v>72</v>
+      </c>
+      <c r="R8" s="2">
+        <v>113418617</v>
+      </c>
+      <c r="S8">
+        <v>1.01456179356613</v>
+      </c>
+      <c r="T8">
+        <v>1.0502401690701999</v>
+      </c>
+      <c r="U8" s="2">
+        <v>119116787.493789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>37256</v>
       </c>
@@ -2868,8 +3198,26 @@
       <c r="E9">
         <v>1.0317713151585</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P9" s="10">
+        <v>37256</v>
+      </c>
+      <c r="Q9">
+        <v>60</v>
+      </c>
+      <c r="R9" s="2">
+        <v>120298776</v>
+      </c>
+      <c r="S9">
+        <v>1.01955362337227</v>
+      </c>
+      <c r="T9">
+        <v>1.07077616978663</v>
+      </c>
+      <c r="U9" s="2">
+        <v>128813062.5953</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>37621</v>
       </c>
@@ -2882,8 +3230,26 @@
       <c r="D10">
         <v>1.06338854293367</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P10" s="10">
+        <v>37621</v>
+      </c>
+      <c r="Q10">
+        <v>48</v>
+      </c>
+      <c r="R10" s="2">
+        <v>111774418</v>
+      </c>
+      <c r="S10">
+        <v>1.0297559094086799</v>
+      </c>
+      <c r="T10">
+        <v>1.1026380884917799</v>
+      </c>
+      <c r="U10" s="2">
+        <v>123246730.605801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>37986</v>
       </c>
@@ -2893,23 +3259,88 @@
       <c r="C11">
         <v>1.1721053090090801</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P11" s="10">
+        <v>37986</v>
+      </c>
+      <c r="Q11">
+        <v>36</v>
+      </c>
+      <c r="R11" s="2">
+        <v>130480200</v>
+      </c>
+      <c r="S11">
+        <v>1.0566080746314901</v>
+      </c>
+      <c r="T11">
+        <v>1.16505630769665</v>
+      </c>
+      <c r="U11" s="2">
+        <v>152016780.03952101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>38352</v>
       </c>
       <c r="B12">
         <v>1.61866550511115</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P12" s="10">
+        <v>38352</v>
+      </c>
+      <c r="Q12">
+        <v>24</v>
+      </c>
+      <c r="R12" s="2">
+        <v>100442115</v>
+      </c>
+      <c r="S12">
+        <v>1.1437721330327499</v>
+      </c>
+      <c r="T12">
+        <v>1.3325589381574601</v>
+      </c>
+      <c r="U12" s="2">
+        <v>133845038.110689</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>38717</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P13" s="10">
+        <v>38717</v>
+      </c>
+      <c r="Q13">
+        <v>12</v>
+      </c>
+      <c r="R13" s="2">
+        <v>68388763</v>
+      </c>
+      <c r="S13">
+        <v>1.6245863032932999</v>
+      </c>
+      <c r="T13">
+        <v>2.1648569992616702</v>
+      </c>
+      <c r="U13" s="2">
+        <v>148051892.25139701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1306876488</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1476812135.2927001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>1.6245863032932999</v>
@@ -2945,9 +3376,9 @@
         <v>1.0033341793686099</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>1.64767558586787</v>
@@ -2985,7 +3416,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>1.6465734975053701</v>
@@ -3023,7 +3454,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>1.63944020094222</v>
@@ -3055,7 +3486,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>1.6483747738296199</v>
@@ -3093,7 +3524,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21">
         <v>1.6245863032932999</v>
@@ -3131,7 +3562,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -3139,7 +3570,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>1.6245863032932999</v>
@@ -3180,7 +3611,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>2.1648569992616702</v>
@@ -3221,7 +3652,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>0.46192427506345801</v>
@@ -3307,14 +3738,14 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="13">
-        <f ca="1">+OFFSET($B$34,B28,0)</f>
+        <f ca="1">+OFFSET($B$35,B28,0)</f>
         <v>1.6245863032932999</v>
       </c>
       <c r="C29" s="13">
-        <f t="shared" ref="C29:L29" ca="1" si="1">+OFFSET($B$34,C28,0)</f>
+        <f t="shared" ref="C29:L29" ca="1" si="1">+OFFSET($B$35,C28,0)</f>
         <v>1.1437721330327399</v>
       </c>
       <c r="D29" s="13">
@@ -3356,7 +3787,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="13">
         <f t="shared" ref="B30:I30" si="2">+B15</f>
@@ -3449,106 +3880,159 @@
         <v>-9.9920072216264089E-15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33">
+        <f>1/B24</f>
+        <v>0.61554132148771523</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:M33" si="5">1/C24</f>
+        <v>0.87430002106142124</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="5"/>
+        <v>0.94642471888052426</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="5"/>
+        <v>0.97110391973786614</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="5"/>
+        <v>0.98082138798389584</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>0.9856472088161865</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="5"/>
+        <v>0.98893713374292325</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="5"/>
+        <v>0.99197939149894143</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>0.99289321959936006</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="5"/>
+        <v>0.99508826916458937</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="5"/>
+        <v>0.99667690044137824</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="B35" s="12">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="12">
         <v>1.6245863032932999</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <f>1+A35</f>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <f>1+A36</f>
         <v>2</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B37" s="12">
         <v>1.1437721330327399</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <f t="shared" ref="A37:A45" si="5">1+A36</f>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <f t="shared" ref="A38:A46" si="6">1+A37</f>
         <v>3</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B38" s="12">
         <v>1.0566080746314901</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <f t="shared" si="5"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B39" s="12">
         <v>1.0297559094086799</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <f t="shared" si="5"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B40" s="12">
         <v>1.01955362337227</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <f t="shared" si="5"/>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B41" s="12">
         <v>1.01456179356613</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <f t="shared" si="5"/>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B42" s="12">
         <v>1.0111866223641599</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <f t="shared" si="5"/>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B43" s="12">
         <v>1.00808545880064</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <f t="shared" si="5"/>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B44" s="12">
         <v>1.0071576482348299</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <f t="shared" si="5"/>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B45" s="12">
         <v>1.00493597501609</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <f t="shared" si="5"/>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B46" s="12">
         <v>1.0033341793685999</v>
       </c>
     </row>
@@ -3562,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3582,33 +4066,33 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>55</v>
-      </c>
-      <c r="N1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" t="str">
         <f>+E2</f>

</xml_diff>

<commit_message>
udpated claims data (reserving)
</commit_message>
<xml_diff>
--- a/data/reservingAccident/triangle.xlsx
+++ b/data/reservingAccident/triangle.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="63">
   <si>
     <t>NA</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Ratio to Ultimate</t>
   </si>
   <si>
-    <t>Ultimate Based on Y2</t>
-  </si>
-  <si>
-    <t>Delta to Ultimate based on Diag</t>
-  </si>
-  <si>
     <t>AccidentYear––––– </t>
   </si>
   <si>
@@ -216,9 +210,6 @@
   </si>
   <si>
     <t>UltimateLoss(2) x (4)–––––(5)</t>
-  </si>
-  <si>
-    <t>12-24</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3:AB14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1105,12 +1098,12 @@
         <v>1</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
@@ -1151,13 +1144,13 @@
         <v>12</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>2</v>
@@ -1169,52 +1162,46 @@
         <v>5</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.35">
@@ -1225,40 +1212,40 @@
         <v>1</v>
       </c>
       <c r="C4" s="9">
-        <v>54528825</v>
+        <v>34098350</v>
       </c>
       <c r="D4" s="9">
-        <v>84930173</v>
+        <v>52156557</v>
       </c>
       <c r="E4" s="9">
-        <v>95155175</v>
+        <v>59729692</v>
       </c>
       <c r="F4" s="9">
-        <v>100076635</v>
+        <v>63358838</v>
       </c>
       <c r="G4" s="9">
-        <v>102745306</v>
+        <v>65597261</v>
       </c>
       <c r="H4" s="9">
-        <v>104782943</v>
+        <v>67157805</v>
       </c>
       <c r="I4" s="9">
-        <v>106243585</v>
+        <v>68266214</v>
       </c>
       <c r="J4" s="9">
-        <v>107327580</v>
+        <v>69174506</v>
       </c>
       <c r="K4" s="9">
-        <v>108006131</v>
+        <v>69835594</v>
       </c>
       <c r="L4" s="9">
-        <v>108593649</v>
+        <v>70357772</v>
       </c>
       <c r="M4" s="9">
-        <v>109030127</v>
+        <v>70777164</v>
       </c>
       <c r="N4" s="9">
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="P4" s="5">
         <f>+truth!A3</f>
@@ -1266,11 +1253,11 @@
       </c>
       <c r="Q4" s="5">
         <f>+T4+P4</f>
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="R4" s="5">
         <f>+AE4</f>
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="S4" s="5">
         <f>+AK4</f>
@@ -1278,7 +1265,7 @@
       </c>
       <c r="T4" s="5">
         <f>+AI4</f>
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="U4" s="4">
         <f t="shared" ref="U4:U15" si="0">+T4/R4</f>
@@ -1301,31 +1288,23 @@
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B4)-U4</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="2">
-        <f t="shared" ref="AA4:AA14" si="2">+D4/$U$14</f>
-        <v>113174461.15040897</v>
-      </c>
-      <c r="AB4" s="2">
-        <f t="shared" ref="AB4:AB14" si="3">+R4-AA4</f>
-        <v>-3780808.1504089683</v>
-      </c>
       <c r="AD4" s="7">
         <v>34699</v>
       </c>
       <c r="AE4" s="8">
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="AF4" s="8">
         <v>1</v>
       </c>
       <c r="AG4" s="8">
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="AH4" s="8">
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="AI4" s="8">
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="AJ4" s="8">
         <v>0</v>
@@ -1347,159 +1326,151 @@
         <v>2</v>
       </c>
       <c r="C5" s="9">
-        <v>52617643</v>
+        <v>32651698</v>
       </c>
       <c r="D5" s="9">
-        <v>82326081</v>
+        <v>49466503</v>
       </c>
       <c r="E5" s="9">
-        <v>92488762</v>
+        <v>55681931</v>
       </c>
       <c r="F5" s="9">
-        <v>97083953</v>
+        <v>59197484</v>
       </c>
       <c r="G5" s="9">
-        <v>99779085</v>
+        <v>61414330</v>
       </c>
       <c r="H5" s="9">
-        <v>101642338</v>
+        <v>62802514</v>
       </c>
       <c r="I5" s="9">
-        <v>103048081</v>
+        <v>63779033</v>
       </c>
       <c r="J5" s="9">
-        <v>104144626</v>
+        <v>64549839</v>
       </c>
       <c r="K5" s="9">
-        <v>104930498</v>
+        <v>65275539</v>
       </c>
       <c r="L5" s="9">
-        <v>105694105</v>
+        <v>65802502</v>
       </c>
       <c r="M5" s="9">
-        <v>106315346</v>
+        <v>66282796</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="P5" s="5">
         <f>+truth!A4</f>
-        <v>402632</v>
+        <v>276189</v>
       </c>
       <c r="Q5" s="5">
-        <f t="shared" ref="Q5:Q16" si="4">+T5+P5</f>
-        <v>106717978</v>
+        <f t="shared" ref="Q5:Q16" si="2">+T5+P5</f>
+        <v>66558985</v>
       </c>
       <c r="R5" s="5">
-        <f t="shared" ref="R5:R15" si="5">+AE5</f>
-        <v>106669820.4332</v>
+        <f t="shared" ref="R5:R15" si="3">+AE5</f>
+        <v>66619385.246157899</v>
       </c>
       <c r="S5" s="5">
-        <f t="shared" ref="S5:S15" si="6">+AK5</f>
-        <v>354474.433199525</v>
+        <f t="shared" ref="S5:S15" si="4">+AK5</f>
+        <v>336589.24615787697</v>
       </c>
       <c r="T5" s="5">
-        <f t="shared" ref="T5:T15" si="7">+AI5</f>
-        <v>106315346</v>
+        <f t="shared" ref="T5:T15" si="5">+AI5</f>
+        <v>66282796</v>
       </c>
       <c r="U5" s="4">
         <f t="shared" si="0"/>
-        <v>0.99667690044137658</v>
+        <v>0.99494757802230982</v>
       </c>
       <c r="V5" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B5)</f>
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
       <c r="W5" s="4">
-        <f t="shared" ref="W5:W15" ca="1" si="8">1/V5</f>
-        <v>0.99667690044137824</v>
+        <f t="shared" ref="W5:W15" ca="1" si="6">1/V5</f>
+        <v>0.99494757802230904</v>
       </c>
       <c r="X5" s="16">
-        <f t="shared" ref="X5:X15" ca="1" si="9">+OFFSET($N5,0,-B5+1)-T5</f>
+        <f t="shared" ref="X5:X15" ca="1" si="7">+OFFSET($N5,0,-B5+1)-T5</f>
         <v>0</v>
       </c>
       <c r="Y5" s="15">
         <f>+R5-S5-T5</f>
-        <v>4.76837158203125E-7</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B5)-U5</f>
-        <v>4.4408920985006262E-15</v>
-      </c>
-      <c r="AA5" s="2">
-        <f t="shared" si="2"/>
-        <v>109704355.08002464</v>
-      </c>
-      <c r="AB5" s="2">
-        <f t="shared" si="3"/>
-        <v>-3034534.646824643</v>
+        <v>0</v>
       </c>
       <c r="AD5" s="7">
         <v>35064</v>
       </c>
       <c r="AE5" s="8">
-        <v>106669820.4332</v>
+        <v>66619385.246157899</v>
       </c>
       <c r="AF5" s="8">
         <v>1</v>
       </c>
       <c r="AG5" s="8">
-        <v>106669820.4332</v>
+        <v>66619385.246157899</v>
       </c>
       <c r="AH5" s="8">
-        <v>106315346</v>
+        <v>66282796</v>
       </c>
       <c r="AI5" s="8">
-        <v>106315346</v>
+        <v>66282796</v>
       </c>
       <c r="AJ5" s="8">
         <v>0</v>
       </c>
       <c r="AK5" s="8">
-        <v>354474.433199525</v>
+        <v>336589.24615787697</v>
       </c>
       <c r="AL5" s="8">
-        <v>354474.433199525</v>
+        <v>336589.24615787697</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" ref="A6:A15" si="10">+A5+1</f>
+        <f t="shared" ref="A6:A15" si="8">+A5+1</f>
         <v>1996</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B15" si="11">1+B5</f>
+        <f t="shared" ref="B6:B15" si="9">1+B5</f>
         <v>3</v>
       </c>
       <c r="C6" s="9">
-        <v>52802533</v>
+        <v>34960516</v>
       </c>
       <c r="D6" s="9">
-        <v>83811749</v>
+        <v>55485220</v>
       </c>
       <c r="E6" s="9">
-        <v>96639642</v>
+        <v>63903664</v>
       </c>
       <c r="F6" s="9">
-        <v>102574259</v>
+        <v>68268004</v>
       </c>
       <c r="G6" s="9">
-        <v>106289046</v>
+        <v>71066045</v>
       </c>
       <c r="H6" s="9">
-        <v>108676563</v>
+        <v>73098108</v>
       </c>
       <c r="I6" s="9">
-        <v>110653125</v>
+        <v>74668974</v>
       </c>
       <c r="J6" s="9">
-        <v>111962351</v>
+        <v>75891430</v>
       </c>
       <c r="K6" s="9">
-        <v>112911041</v>
+        <v>76823786</v>
       </c>
       <c r="L6" s="9">
-        <v>113892219</v>
+        <v>77530054</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>0</v>
@@ -1509,119 +1480,111 @@
       </c>
       <c r="P6" s="5">
         <f>+truth!A5</f>
-        <v>1362840</v>
+        <v>822196</v>
       </c>
       <c r="Q6" s="5">
+        <f t="shared" si="2"/>
+        <v>78352250</v>
+      </c>
+      <c r="R6" s="5">
+        <f t="shared" si="3"/>
+        <v>78438642.935137793</v>
+      </c>
+      <c r="S6" s="5">
         <f t="shared" si="4"/>
-        <v>115255059</v>
-      </c>
-      <c r="R6" s="5">
+        <v>908588.93513780797</v>
+      </c>
+      <c r="T6" s="5">
         <f t="shared" si="5"/>
-        <v>114835999.60712001</v>
-      </c>
-      <c r="S6" s="5">
-        <f t="shared" si="6"/>
-        <v>943780.60712005198</v>
-      </c>
-      <c r="T6" s="5">
-        <f t="shared" si="7"/>
-        <v>113892219</v>
+        <v>77530054</v>
       </c>
       <c r="U6" s="4">
         <f t="shared" si="0"/>
-        <v>0.99178149177654307</v>
+        <v>0.9884165648315828</v>
       </c>
       <c r="V6" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B6)</f>
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="W6" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.99508826916458937</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.99343582181112344</v>
       </c>
       <c r="X6" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y6" s="15">
-        <f t="shared" ref="Y6:Y15" si="12">+R6-S6-T6</f>
+        <f t="shared" ref="Y6:Y15" si="10">+R6-S6-T6</f>
         <v>0</v>
       </c>
       <c r="Z6" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B6)-U6</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="2">
-        <f t="shared" si="2"/>
-        <v>111684095.25255916</v>
-      </c>
-      <c r="AB6" s="2">
-        <f t="shared" si="3"/>
-        <v>3151904.3545608521</v>
-      </c>
       <c r="AD6" s="7">
         <v>35430</v>
       </c>
       <c r="AE6" s="8">
-        <v>114835999.60712001</v>
+        <v>78438642.935137793</v>
       </c>
       <c r="AF6" s="8">
         <v>1</v>
       </c>
       <c r="AG6" s="8">
-        <v>114835999.60712001</v>
+        <v>78438642.935137793</v>
       </c>
       <c r="AH6" s="8">
-        <v>113892219</v>
+        <v>77530054</v>
       </c>
       <c r="AI6" s="8">
-        <v>113892219</v>
+        <v>77530054</v>
       </c>
       <c r="AJ6" s="8">
         <v>0</v>
       </c>
       <c r="AK6" s="8">
-        <v>943780.60712005198</v>
+        <v>908588.93513780797</v>
       </c>
       <c r="AL6" s="8">
-        <v>943780.60712005198</v>
+        <v>908588.93513780797</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1997</v>
       </c>
       <c r="B7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="C7" s="9">
-        <v>49838540</v>
+        <v>32109764</v>
       </c>
       <c r="D7" s="9">
-        <v>80421914</v>
+        <v>50301337</v>
       </c>
       <c r="E7" s="9">
-        <v>91873925</v>
+        <v>56922184</v>
       </c>
       <c r="F7" s="9">
-        <v>96987472</v>
+        <v>60421087</v>
       </c>
       <c r="G7" s="9">
-        <v>99474577</v>
+        <v>62600742</v>
       </c>
       <c r="H7" s="9">
-        <v>101271088</v>
+        <v>64147676</v>
       </c>
       <c r="I7" s="9">
-        <v>102774844</v>
+        <v>65267989</v>
       </c>
       <c r="J7" s="9">
-        <v>103992270</v>
+        <v>66194157</v>
       </c>
       <c r="K7" s="9">
-        <v>105035099</v>
+        <v>66936974</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>0</v>
@@ -1634,116 +1597,108 @@
       </c>
       <c r="P7" s="5">
         <f>+truth!A6</f>
-        <v>2052225</v>
+        <v>1484528</v>
       </c>
       <c r="Q7" s="5">
+        <f t="shared" si="2"/>
+        <v>68421502</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" si="3"/>
+        <v>68282341.896776706</v>
+      </c>
+      <c r="S7" s="5">
         <f t="shared" si="4"/>
-        <v>107087324</v>
-      </c>
-      <c r="R7" s="5">
+        <v>1345367.89677672</v>
+      </c>
+      <c r="T7" s="5">
         <f t="shared" si="5"/>
-        <v>106663518.29318801</v>
-      </c>
-      <c r="S7" s="5">
-        <f t="shared" si="6"/>
-        <v>1628419.29318833</v>
-      </c>
-      <c r="T7" s="5">
-        <f t="shared" si="7"/>
-        <v>105035099</v>
+        <v>66936974</v>
       </c>
       <c r="U7" s="4">
         <f t="shared" si="0"/>
-        <v>0.98473311850906753</v>
+        <v>0.9802969866087704</v>
       </c>
       <c r="V7" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B7)</f>
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="W7" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.99289321959936006</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.99178526694947211</v>
       </c>
       <c r="X7" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y7" s="15">
-        <f t="shared" si="12"/>
-        <v>-3.2782554626464844E-7</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Z7" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B7)-U7</f>
-        <v>-2.55351295663786E-15</v>
-      </c>
-      <c r="AA7" s="2">
-        <f t="shared" si="2"/>
-        <v>107166940.32443018</v>
-      </c>
-      <c r="AB7" s="2">
-        <f t="shared" si="3"/>
-        <v>-503422.03124217689</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="7">
         <v>35795</v>
       </c>
       <c r="AE7" s="8">
-        <v>106663518.29318801</v>
+        <v>68282341.896776706</v>
       </c>
       <c r="AF7" s="8">
         <v>1</v>
       </c>
       <c r="AG7" s="8">
-        <v>106663518.29318801</v>
+        <v>68282341.896776706</v>
       </c>
       <c r="AH7" s="8">
-        <v>105035099</v>
+        <v>66936974</v>
       </c>
       <c r="AI7" s="8">
-        <v>105035099</v>
+        <v>66936974</v>
       </c>
       <c r="AJ7" s="8">
         <v>0</v>
       </c>
       <c r="AK7" s="8">
-        <v>1628419.29318833</v>
+        <v>1345367.89677672</v>
       </c>
       <c r="AL7" s="8">
-        <v>1628419.29318833</v>
+        <v>1345367.89677672</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1998</v>
       </c>
       <c r="B8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="C8" s="9">
-        <v>52703836</v>
+        <v>33437081</v>
       </c>
       <c r="D8" s="9">
-        <v>86610906</v>
+        <v>53130343</v>
       </c>
       <c r="E8" s="9">
-        <v>97974767</v>
+        <v>61071087</v>
       </c>
       <c r="F8" s="9">
-        <v>103425365</v>
+        <v>65227876</v>
       </c>
       <c r="G8" s="9">
-        <v>106515923</v>
+        <v>67967792</v>
       </c>
       <c r="H8" s="9">
-        <v>108683986</v>
+        <v>69698504</v>
       </c>
       <c r="I8" s="9">
-        <v>110216385</v>
+        <v>70861094</v>
       </c>
       <c r="J8" s="9">
-        <v>111470947</v>
+        <v>71925937</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>0</v>
@@ -1759,113 +1714,105 @@
       </c>
       <c r="P8" s="5">
         <f>+truth!A7</f>
-        <v>2932050</v>
+        <v>1991356</v>
       </c>
       <c r="Q8" s="5">
+        <f t="shared" si="2"/>
+        <v>73917293</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="3"/>
+        <v>74186127.936697498</v>
+      </c>
+      <c r="S8" s="5">
         <f t="shared" si="4"/>
-        <v>114402997</v>
-      </c>
-      <c r="R8" s="5">
+        <v>2260190.9366974798</v>
+      </c>
+      <c r="T8" s="5">
         <f t="shared" si="5"/>
-        <v>114114411.953134</v>
-      </c>
-      <c r="S8" s="5">
-        <f t="shared" si="6"/>
-        <v>2643464.9531339598</v>
-      </c>
-      <c r="T8" s="5">
-        <f t="shared" si="7"/>
-        <v>111470947</v>
+        <v>71925937</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" si="0"/>
-        <v>0.9768349596874788</v>
+        <v>0.9695335098412724</v>
       </c>
       <c r="V8" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B8)</f>
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="W8" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.99197939149894143</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.98902018784661183</v>
       </c>
       <c r="X8" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y8" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z8" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B8)-U8</f>
         <v>0</v>
       </c>
-      <c r="AA8" s="2">
-        <f t="shared" si="2"/>
-        <v>115414136.93221517</v>
-      </c>
-      <c r="AB8" s="2">
-        <f t="shared" si="3"/>
-        <v>-1299724.9790811688</v>
-      </c>
       <c r="AD8" s="7">
         <v>36160</v>
       </c>
       <c r="AE8" s="8">
-        <v>114114411.953134</v>
+        <v>74186127.936697498</v>
       </c>
       <c r="AF8" s="8">
         <v>1</v>
       </c>
       <c r="AG8" s="8">
-        <v>114114411.953134</v>
+        <v>74186127.936697498</v>
       </c>
       <c r="AH8" s="8">
-        <v>111470947</v>
+        <v>71925937</v>
       </c>
       <c r="AI8" s="8">
-        <v>111470947</v>
+        <v>71925937</v>
       </c>
       <c r="AJ8" s="8">
         <v>0</v>
       </c>
       <c r="AK8" s="8">
-        <v>2643464.9531339598</v>
+        <v>2260190.9366974798</v>
       </c>
       <c r="AL8" s="8">
-        <v>2643464.9531339598</v>
+        <v>2260190.9366974798</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1999</v>
       </c>
       <c r="B9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="C9" s="9">
-        <v>53858548</v>
+        <v>32093915</v>
       </c>
       <c r="D9" s="9">
-        <v>89297134</v>
+        <v>50994601</v>
       </c>
       <c r="E9" s="9">
-        <v>103023703</v>
+        <v>58269456</v>
       </c>
       <c r="F9" s="9">
-        <v>109080056</v>
+        <v>62067387</v>
       </c>
       <c r="G9" s="9">
-        <v>112420272</v>
+        <v>64465682</v>
       </c>
       <c r="H9" s="9">
-        <v>114531877</v>
+        <v>66044718</v>
       </c>
       <c r="I9" s="9">
-        <v>115966335</v>
+        <v>67271819</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>0</v>
@@ -1884,110 +1831,102 @@
       </c>
       <c r="P9" s="5">
         <f>+truth!A8</f>
-        <v>3760055</v>
+        <v>2893142</v>
       </c>
       <c r="Q9" s="5">
+        <f t="shared" si="2"/>
+        <v>70164961</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="3"/>
+        <v>70375933.015466496</v>
+      </c>
+      <c r="S9" s="5">
         <f t="shared" si="4"/>
-        <v>119726390</v>
-      </c>
-      <c r="R9" s="5">
+        <v>3104114.0154664698</v>
+      </c>
+      <c r="T9" s="5">
         <f t="shared" si="5"/>
-        <v>120044440.909565</v>
-      </c>
-      <c r="S9" s="5">
-        <f t="shared" si="6"/>
-        <v>4078105.90956512</v>
-      </c>
-      <c r="T9" s="5">
-        <f t="shared" si="7"/>
-        <v>115966335</v>
+        <v>67271819</v>
       </c>
       <c r="U9" s="4">
         <f t="shared" si="0"/>
-        <v>0.96602836517321755</v>
+        <v>0.95589239271919413</v>
       </c>
       <c r="V9" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B9)</f>
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="W9" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.98893713374292325</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.98593022625457094</v>
       </c>
       <c r="X9" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y9" s="15">
-        <f t="shared" si="12"/>
-        <v>-1.1920928955078125E-7</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Z9" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B9)-U9</f>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="2">
-        <f t="shared" si="2"/>
-        <v>118993694.06354399</v>
-      </c>
-      <c r="AB9" s="2">
-        <f t="shared" si="3"/>
-        <v>1050746.8460210115</v>
+        <v>8.8817841970012523E-16</v>
       </c>
       <c r="AD9" s="7">
         <v>36525</v>
       </c>
       <c r="AE9" s="8">
-        <v>120044440.909565</v>
+        <v>70375933.015466496</v>
       </c>
       <c r="AF9" s="8">
         <v>1</v>
       </c>
       <c r="AG9" s="8">
-        <v>120044440.909565</v>
+        <v>70375933.015466496</v>
       </c>
       <c r="AH9" s="8">
-        <v>115966335</v>
+        <v>67271819</v>
       </c>
       <c r="AI9" s="8">
-        <v>115966335</v>
+        <v>67271819</v>
       </c>
       <c r="AJ9" s="8">
         <v>0</v>
       </c>
       <c r="AK9" s="8">
-        <v>4078105.90956512</v>
+        <v>3104114.0154664698</v>
       </c>
       <c r="AL9" s="8">
-        <v>4078105.90956512</v>
+        <v>3104114.0154664698</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2000</v>
       </c>
       <c r="B10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="C10" s="9">
-        <v>54694527</v>
+        <v>33147688</v>
       </c>
       <c r="D10" s="9">
-        <v>90220052</v>
+        <v>52850049</v>
       </c>
       <c r="E10" s="9">
-        <v>102634248</v>
+        <v>60064330</v>
       </c>
       <c r="F10" s="9">
-        <v>108224574</v>
+        <v>63548230</v>
       </c>
       <c r="G10" s="9">
-        <v>111341566</v>
+        <v>65538698</v>
       </c>
       <c r="H10" s="9">
-        <v>113418617</v>
+        <v>66996567</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>0</v>
@@ -2009,107 +1948,99 @@
       </c>
       <c r="P10" s="5">
         <f>+truth!A9</f>
-        <v>5584206</v>
+        <v>3652487</v>
       </c>
       <c r="Q10" s="5">
+        <f t="shared" si="2"/>
+        <v>70649054</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="3"/>
+        <v>71334380.768883795</v>
+      </c>
+      <c r="S10" s="5">
         <f t="shared" si="4"/>
-        <v>119002823</v>
-      </c>
-      <c r="R10" s="5">
+        <v>4337813.7688837899</v>
+      </c>
+      <c r="T10" s="5">
         <f t="shared" si="5"/>
-        <v>119116787.493789</v>
-      </c>
-      <c r="S10" s="5">
-        <f t="shared" si="6"/>
-        <v>5698170.4937885301</v>
-      </c>
-      <c r="T10" s="5">
-        <f t="shared" si="7"/>
-        <v>113418617</v>
+        <v>66996567</v>
       </c>
       <c r="U10" s="4">
         <f t="shared" si="0"/>
-        <v>0.95216316177024063</v>
+        <v>0.93919041951260673</v>
       </c>
       <c r="V10" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B10)</f>
-        <v>1.01456179356613</v>
+        <v>1.01778337263625</v>
       </c>
       <c r="W10" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.9856472088161865</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.98252735000947433</v>
       </c>
       <c r="X10" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y10" s="15">
-        <f t="shared" si="12"/>
-        <v>4.76837158203125E-7</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Z10" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B10)-U10</f>
-        <v>4.3298697960381105E-15</v>
-      </c>
-      <c r="AA10" s="2">
-        <f t="shared" si="2"/>
-        <v>120223536.69363038</v>
-      </c>
-      <c r="AB10" s="2">
-        <f t="shared" si="3"/>
-        <v>-1106749.1998413801</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="7">
         <v>36891</v>
       </c>
       <c r="AE10" s="8">
-        <v>119116787.493789</v>
+        <v>71334380.768883795</v>
       </c>
       <c r="AF10" s="8">
         <v>1</v>
       </c>
       <c r="AG10" s="8">
-        <v>119116787.493789</v>
+        <v>71334380.768883795</v>
       </c>
       <c r="AH10" s="8">
-        <v>113418617</v>
+        <v>66996567</v>
       </c>
       <c r="AI10" s="8">
-        <v>113418617</v>
+        <v>66996567</v>
       </c>
       <c r="AJ10" s="8">
         <v>0</v>
       </c>
       <c r="AK10" s="8">
-        <v>5698170.4937885301</v>
+        <v>4337813.7688837899</v>
       </c>
       <c r="AL10" s="8">
-        <v>5698170.4937885301</v>
+        <v>4337813.7688837899</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2001</v>
       </c>
       <c r="B11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="C11" s="9">
-        <v>58603881</v>
+        <v>34094566</v>
       </c>
       <c r="D11" s="9">
-        <v>96002420</v>
+        <v>54527704</v>
       </c>
       <c r="E11" s="9">
-        <v>110246744</v>
+        <v>62666406</v>
       </c>
       <c r="F11" s="9">
-        <v>116594418</v>
+        <v>66995865</v>
       </c>
       <c r="G11" s="9">
-        <v>120298776</v>
+        <v>69639352</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>0</v>
@@ -2134,104 +2065,96 @@
       </c>
       <c r="P11" s="5">
         <f>+truth!A10</f>
-        <v>7233582</v>
+        <v>5656252</v>
       </c>
       <c r="Q11" s="5">
+        <f t="shared" si="2"/>
+        <v>75295604</v>
+      </c>
+      <c r="R11" s="5">
+        <f t="shared" si="3"/>
+        <v>75974352.335073903</v>
+      </c>
+      <c r="S11" s="5">
         <f t="shared" si="4"/>
-        <v>127532358</v>
-      </c>
-      <c r="R11" s="5">
+        <v>6335000.3350739302</v>
+      </c>
+      <c r="T11" s="5">
         <f t="shared" si="5"/>
-        <v>128813062.5953</v>
-      </c>
-      <c r="S11" s="5">
-        <f t="shared" si="6"/>
-        <v>8514286.5953000207</v>
-      </c>
-      <c r="T11" s="5">
-        <f t="shared" si="7"/>
-        <v>120298776</v>
+        <v>69639352</v>
       </c>
       <c r="U11" s="4">
         <f t="shared" si="0"/>
-        <v>0.93390199391462447</v>
+        <v>0.91661659309533439</v>
       </c>
       <c r="V11" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B11)</f>
-        <v>1.01955362337227</v>
+        <v>1.0246273377411199</v>
       </c>
       <c r="W11" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.98082138798389584</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.97596459040863281</v>
       </c>
       <c r="X11" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y11" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z11" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B11)-U11</f>
         <v>0</v>
       </c>
-      <c r="AA11" s="2">
-        <f t="shared" si="2"/>
-        <v>127928882.85574603</v>
-      </c>
-      <c r="AB11" s="2">
-        <f t="shared" si="3"/>
-        <v>884179.73955397308</v>
-      </c>
       <c r="AD11" s="7">
         <v>37256</v>
       </c>
       <c r="AE11" s="8">
-        <v>128813062.5953</v>
+        <v>75974352.335073903</v>
       </c>
       <c r="AF11" s="8">
         <v>1</v>
       </c>
       <c r="AG11" s="8">
-        <v>128813062.5953</v>
+        <v>75974352.335073903</v>
       </c>
       <c r="AH11" s="8">
-        <v>120298776</v>
+        <v>69639352</v>
       </c>
       <c r="AI11" s="8">
-        <v>120298776</v>
+        <v>69639352</v>
       </c>
       <c r="AJ11" s="8">
         <v>0</v>
       </c>
       <c r="AK11" s="8">
-        <v>8514286.5953000207</v>
+        <v>6335000.3350739302</v>
       </c>
       <c r="AL11" s="8">
-        <v>8514286.5953000207</v>
+        <v>6335000.3350739302</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2002</v>
       </c>
       <c r="B12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="C12" s="9">
-        <v>56264364</v>
+        <v>35042399</v>
       </c>
       <c r="D12" s="9">
-        <v>91765553</v>
+        <v>56369050</v>
       </c>
       <c r="E12" s="9">
-        <v>105111550</v>
+        <v>64928517</v>
       </c>
       <c r="F12" s="9">
-        <v>111774418</v>
+        <v>69554382</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>0</v>
@@ -2259,101 +2182,93 @@
       </c>
       <c r="P12" s="5">
         <f>+truth!A11</f>
-        <v>12818962</v>
+        <v>8988414</v>
       </c>
       <c r="Q12" s="5">
+        <f t="shared" si="2"/>
+        <v>78542796</v>
+      </c>
+      <c r="R12" s="5">
+        <f t="shared" si="3"/>
+        <v>78744274.363945693</v>
+      </c>
+      <c r="S12" s="5">
         <f t="shared" si="4"/>
-        <v>124593380</v>
-      </c>
-      <c r="R12" s="5">
+        <v>9189892.3639457095</v>
+      </c>
+      <c r="T12" s="5">
         <f t="shared" si="5"/>
-        <v>123246730.605801</v>
-      </c>
-      <c r="S12" s="5">
-        <f t="shared" si="6"/>
-        <v>11472312.6058012</v>
-      </c>
-      <c r="T12" s="5">
-        <f t="shared" si="7"/>
-        <v>111774418</v>
+        <v>69554382</v>
       </c>
       <c r="U12" s="4">
         <f t="shared" si="0"/>
-        <v>0.90691588694149894</v>
+        <v>0.88329446885914242</v>
       </c>
       <c r="V12" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B12)</f>
-        <v>1.0297559094086799</v>
+        <v>1.03772481931108</v>
       </c>
       <c r="W12" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.97110391973786614</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.96364660591222584</v>
       </c>
       <c r="X12" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y12" s="15">
-        <f t="shared" si="12"/>
-        <v>-1.9371509552001953E-7</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Z12" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B12)-U12</f>
-        <v>-8.8817841970012523E-16</v>
-      </c>
-      <c r="AA12" s="2">
-        <f t="shared" si="2"/>
-        <v>122283007.86511168</v>
-      </c>
-      <c r="AB12" s="2">
-        <f t="shared" si="3"/>
-        <v>963722.74068932235</v>
+        <v>0</v>
       </c>
       <c r="AD12" s="7">
         <v>37621</v>
       </c>
       <c r="AE12" s="8">
-        <v>123246730.605801</v>
+        <v>78744274.363945693</v>
       </c>
       <c r="AF12" s="8">
         <v>1</v>
       </c>
       <c r="AG12" s="8">
-        <v>123246730.605801</v>
+        <v>78744274.363945693</v>
       </c>
       <c r="AH12" s="8">
-        <v>111774418</v>
+        <v>69554382</v>
       </c>
       <c r="AI12" s="8">
-        <v>111774418</v>
+        <v>69554382</v>
       </c>
       <c r="AJ12" s="8">
         <v>0</v>
       </c>
       <c r="AK12" s="8">
-        <v>11472312.6058012</v>
+        <v>9189892.3639457095</v>
       </c>
       <c r="AL12" s="8">
-        <v>11472312.6058012</v>
+        <v>9189892.3639457095</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2003</v>
       </c>
       <c r="B13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="C13" s="9">
-        <v>65821493</v>
+        <v>36399652</v>
       </c>
       <c r="D13" s="9">
-        <v>111321226</v>
+        <v>58770181</v>
       </c>
       <c r="E13" s="9">
-        <v>130480200</v>
+        <v>66981239</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>0</v>
@@ -2384,98 +2299,90 @@
       </c>
       <c r="P13" s="5">
         <f>+truth!A12</f>
-        <v>24357870</v>
+        <v>11357731</v>
       </c>
       <c r="Q13" s="5">
+        <f t="shared" si="2"/>
+        <v>78338970</v>
+      </c>
+      <c r="R13" s="5">
+        <f t="shared" si="3"/>
+        <v>80772946.658115402</v>
+      </c>
+      <c r="S13" s="5">
         <f t="shared" si="4"/>
-        <v>154838070</v>
-      </c>
-      <c r="R13" s="5">
+        <v>13791707.6581154</v>
+      </c>
+      <c r="T13" s="5">
         <f t="shared" si="5"/>
-        <v>152016780.03952101</v>
-      </c>
-      <c r="S13" s="5">
-        <f t="shared" si="6"/>
-        <v>21536580.039520599</v>
-      </c>
-      <c r="T13" s="5">
-        <f t="shared" si="7"/>
-        <v>130480200</v>
+        <v>66981239</v>
       </c>
       <c r="U13" s="4">
         <f t="shared" si="0"/>
-        <v>0.85832761334688201</v>
+        <v>0.82925337964342138</v>
       </c>
       <c r="V13" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B13)</f>
-        <v>1.0566080746314901</v>
+        <v>1.0651683677659001</v>
       </c>
       <c r="W13" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.94642471888052426</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.93881871661042171</v>
       </c>
       <c r="X13" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y13" s="15">
-        <f t="shared" si="12"/>
-        <v>4.1723251342773438E-7</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Z13" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B13)-U13</f>
-        <v>1.9984014443252818E-15</v>
-      </c>
-      <c r="AA13" s="2">
-        <f t="shared" si="2"/>
-        <v>148342094.71294609</v>
-      </c>
-      <c r="AB13" s="2">
-        <f t="shared" si="3"/>
-        <v>3674685.3265749216</v>
+        <v>0</v>
       </c>
       <c r="AD13" s="7">
         <v>37986</v>
       </c>
       <c r="AE13" s="8">
-        <v>152016780.03952101</v>
+        <v>80772946.658115402</v>
       </c>
       <c r="AF13" s="8">
         <v>1</v>
       </c>
       <c r="AG13" s="8">
-        <v>152016780.03952101</v>
+        <v>80772946.658115402</v>
       </c>
       <c r="AH13" s="8">
-        <v>130480200</v>
+        <v>66981239</v>
       </c>
       <c r="AI13" s="8">
-        <v>130480200</v>
+        <v>66981239</v>
       </c>
       <c r="AJ13" s="8">
         <v>0</v>
       </c>
       <c r="AK13" s="8">
-        <v>21536580.039520599</v>
+        <v>13791707.6581154</v>
       </c>
       <c r="AL13" s="8">
-        <v>21536580.039520599</v>
+        <v>13791707.6581154</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2004</v>
       </c>
       <c r="B14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="C14" s="9">
-        <v>62052422</v>
+        <v>38675116</v>
       </c>
       <c r="D14" s="9">
-        <v>100442115</v>
+        <v>63274548</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>0</v>
@@ -2509,95 +2416,87 @@
       </c>
       <c r="P14" s="5">
         <f>+truth!A13</f>
-        <v>31901613</v>
+        <v>24707983</v>
       </c>
       <c r="Q14" s="5">
+        <f t="shared" si="2"/>
+        <v>87982531</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" si="3"/>
+        <v>87185447.251537502</v>
+      </c>
+      <c r="S14" s="5">
         <f t="shared" si="4"/>
-        <v>132343728</v>
-      </c>
-      <c r="R14" s="5">
+        <v>23910899.251537502</v>
+      </c>
+      <c r="T14" s="5">
         <f t="shared" si="5"/>
-        <v>133845038.110689</v>
-      </c>
-      <c r="S14" s="5">
-        <f t="shared" si="6"/>
-        <v>33402923.1106891</v>
-      </c>
-      <c r="T14" s="5">
-        <f t="shared" si="7"/>
-        <v>100442115</v>
+        <v>63274548</v>
       </c>
       <c r="U14" s="4">
         <f t="shared" si="0"/>
-        <v>0.7504358504267824</v>
+        <v>0.72574666982492497</v>
       </c>
       <c r="V14" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B14)</f>
-        <v>1.1437721330327499</v>
+        <v>1.1426209917621299</v>
       </c>
       <c r="W14" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.87430002106142124</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.87518084054960132</v>
       </c>
       <c r="X14" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y14" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z14" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B14)-U14</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="2">
-        <f t="shared" si="2"/>
-        <v>133845038.110689</v>
-      </c>
-      <c r="AB14" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="AD14" s="7">
         <v>38352</v>
       </c>
       <c r="AE14" s="8">
-        <v>133845038.110689</v>
+        <v>87185447.251537502</v>
       </c>
       <c r="AF14" s="8">
         <v>1</v>
       </c>
       <c r="AG14" s="8">
-        <v>133845038.110689</v>
+        <v>87185447.251537502</v>
       </c>
       <c r="AH14" s="8">
-        <v>100442115</v>
+        <v>63274548</v>
       </c>
       <c r="AI14" s="8">
-        <v>100442115</v>
+        <v>63274548</v>
       </c>
       <c r="AJ14" s="8">
         <v>0</v>
       </c>
       <c r="AK14" s="8">
-        <v>33402923.1106891</v>
+        <v>23910899.251537502</v>
       </c>
       <c r="AL14" s="8">
-        <v>33402923.1106891</v>
+        <v>23910899.251537502</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2005</v>
       </c>
       <c r="B15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="C15" s="9">
-        <v>68388763</v>
+        <v>40397929</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>0</v>
@@ -2634,97 +2533,98 @@
       </c>
       <c r="P15" s="5">
         <f>+truth!A14</f>
-        <v>77968325</v>
+        <v>46512588</v>
       </c>
       <c r="Q15" s="5">
+        <f t="shared" si="2"/>
+        <v>86910517</v>
+      </c>
+      <c r="R15" s="5">
+        <f t="shared" si="3"/>
+        <v>88262765.008943394</v>
+      </c>
+      <c r="S15" s="5">
         <f t="shared" si="4"/>
-        <v>146357088</v>
-      </c>
-      <c r="R15" s="5">
+        <v>47864836.008943401</v>
+      </c>
+      <c r="T15" s="5">
         <f t="shared" si="5"/>
-        <v>148051892.25139701</v>
-      </c>
-      <c r="S15" s="5">
-        <f t="shared" si="6"/>
-        <v>79663129.251397505</v>
-      </c>
-      <c r="T15" s="5">
-        <f t="shared" si="7"/>
-        <v>68388763</v>
+        <v>40397929</v>
       </c>
       <c r="U15" s="4">
         <f t="shared" si="0"/>
-        <v>0.46192427506345962</v>
+        <v>0.45770069627783133</v>
       </c>
       <c r="V15" s="4">
         <f ca="1">+OFFSET(LDFs!$A$26,-11,13-B15)</f>
-        <v>1.6245863032932999</v>
+        <v>1.5856359313563</v>
       </c>
       <c r="W15" s="4">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.61554132148771523</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.63066179330625627</v>
       </c>
       <c r="X15" s="16">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="Y15" s="15">
-        <f t="shared" si="12"/>
-        <v>-4.9173831939697266E-7</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Z15" s="16">
         <f ca="1">+OFFSET(LDFs!$A$26,0,13-B15)-U15</f>
-        <v>-1.609823385706477E-15</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
       <c r="AD15" s="7">
         <v>38717</v>
       </c>
       <c r="AE15" s="8">
-        <v>148051892.25139701</v>
+        <v>88262765.008943394</v>
       </c>
       <c r="AF15" s="8">
         <v>1</v>
       </c>
       <c r="AG15" s="8">
-        <v>148051892.25139701</v>
+        <v>88262765.008943394</v>
       </c>
       <c r="AH15" s="8">
-        <v>68388763</v>
+        <v>40397929</v>
       </c>
       <c r="AI15" s="8">
-        <v>68388763</v>
+        <v>40397929</v>
       </c>
       <c r="AJ15" s="8">
         <v>0</v>
       </c>
       <c r="AK15" s="8">
-        <v>79663129.251397505</v>
+        <v>47864836.008943401</v>
       </c>
       <c r="AL15" s="8">
-        <v>79663129.251397505</v>
+        <v>47864836.008943401</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="P16" s="6">
         <f>+truth!A15</f>
-        <v>170374360</v>
+        <v>108342866</v>
       </c>
       <c r="Q16" s="6">
-        <f t="shared" si="4"/>
-        <v>1477250848</v>
+        <f t="shared" si="2"/>
+        <v>906271039</v>
       </c>
       <c r="R16" s="6">
         <f>+SUM(R4:R15)</f>
-        <v>1476812135.2927041</v>
+        <v>911313173.41673625</v>
       </c>
       <c r="S16" s="6">
         <f>+SUM(S4:S15)</f>
-        <v>169935647.29270393</v>
+        <v>113385000.4167361</v>
       </c>
       <c r="T16" s="6">
         <f>+SUM(T4:T15)</f>
-        <v>1306876488</v>
+        <v>797928173</v>
       </c>
       <c r="X16" s="16">
         <f ca="1">+SUM(X4:X15)</f>
@@ -2732,36 +2632,36 @@
       </c>
       <c r="Y16" s="15">
         <f>+SUM(Y4:Y15)</f>
-        <v>2.384185791015625E-7</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="16">
         <f ca="1">+SUM(Z4:Z15)</f>
-        <v>5.7176485768195562E-15</v>
+        <v>8.8817841970012523E-16</v>
       </c>
       <c r="AD16" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AE16" s="8">
-        <v>1476812135.2927001</v>
+        <v>911313173.41673601</v>
       </c>
       <c r="AF16" s="8"/>
       <c r="AG16" s="8">
-        <v>1476812135.2927001</v>
+        <v>911313173.41673601</v>
       </c>
       <c r="AH16" s="8">
-        <v>1306876488</v>
+        <v>797928173</v>
       </c>
       <c r="AI16" s="8">
-        <v>1306876488</v>
+        <v>797928173</v>
       </c>
       <c r="AJ16" s="8">
         <v>0</v>
       </c>
       <c r="AK16" s="8">
-        <v>169935647.29270399</v>
+        <v>113385000.41673601</v>
       </c>
       <c r="AL16" s="8">
-        <v>169935647.29270399</v>
+        <v>113385000.41673601</v>
       </c>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.35">
@@ -2781,9 +2681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:L24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2796,61 +2694,61 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11">
+        <v>45627</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
       <c r="P1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" t="s">
         <v>60</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>61</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>62</v>
-      </c>
-      <c r="T1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
@@ -2858,37 +2756,37 @@
         <v>34699</v>
       </c>
       <c r="B2">
-        <v>1.55752802302269</v>
+        <v>1.5295918130935999</v>
       </c>
       <c r="C2">
-        <v>1.12039304335339</v>
+        <v>1.1452000560543101</v>
       </c>
       <c r="D2">
-        <v>1.05172036097879</v>
+        <v>1.0607594962987601</v>
       </c>
       <c r="E2">
-        <v>1.02666627430069</v>
+        <v>1.03532929376009</v>
       </c>
       <c r="F2">
-        <v>1.0198319230272199</v>
+        <v>1.0237897737833901</v>
       </c>
       <c r="G2">
-        <v>1.01393969245548</v>
+        <v>1.0165045447807599</v>
       </c>
       <c r="H2">
-        <v>1.01020292189877</v>
+        <v>1.0133051468183101</v>
       </c>
       <c r="I2">
-        <v>1.0063222426146201</v>
+        <v>1.0095568156279999</v>
       </c>
       <c r="J2">
-        <v>1.00543967267932</v>
+        <v>1.0074772472043401</v>
       </c>
       <c r="K2">
-        <v>1.0040193694937001</v>
+        <v>1.0059608482201501</v>
       </c>
       <c r="L2">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
       <c r="P2" s="10">
         <v>34699</v>
@@ -2897,7 +2795,7 @@
         <v>144</v>
       </c>
       <c r="R2" s="2">
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -2906,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="2">
-        <v>109393653</v>
+        <v>71136576</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -2914,34 +2812,34 @@
         <v>35064</v>
       </c>
       <c r="B3">
-        <v>1.5646098210822601</v>
+        <v>1.51497490268347</v>
       </c>
       <c r="C3">
-        <v>1.1234442460585501</v>
+        <v>1.1256492297423999</v>
       </c>
       <c r="D3">
-        <v>1.0496837767165701</v>
+        <v>1.06313633411887</v>
       </c>
       <c r="E3">
-        <v>1.0277608391162201</v>
+        <v>1.03744831452634</v>
       </c>
       <c r="F3">
-        <v>1.0186737831881301</v>
+        <v>1.0226035845380099</v>
       </c>
       <c r="G3">
-        <v>1.01383028989357</v>
+        <v>1.01554904314818</v>
       </c>
       <c r="H3">
-        <v>1.0106411006334</v>
+        <v>1.0120855705040199</v>
       </c>
       <c r="I3">
-        <v>1.0075459678543599</v>
+        <v>1.01124247575583</v>
       </c>
       <c r="J3">
-        <v>1.00727726461376</v>
+        <v>1.0080729015504599</v>
       </c>
       <c r="K3">
-        <v>1.0058777261040199</v>
+        <v>1.00729902337148</v>
       </c>
       <c r="P3" s="10">
         <v>35064</v>
@@ -2950,16 +2848,16 @@
         <v>132</v>
       </c>
       <c r="R3" s="2">
-        <v>106315346</v>
+        <v>66282796</v>
       </c>
       <c r="S3">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
       <c r="T3">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
       <c r="U3" s="2">
-        <v>106669820.4332</v>
+        <v>66619385.246157899</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -2967,31 +2865,31 @@
         <v>35430</v>
       </c>
       <c r="B4">
-        <v>1.5872675843032</v>
+        <v>1.5870824103397101</v>
       </c>
       <c r="C4">
-        <v>1.1530560232074401</v>
+        <v>1.1517240807552001</v>
       </c>
       <c r="D4">
-        <v>1.0614097577058501</v>
+        <v>1.0682956144736899</v>
       </c>
       <c r="E4">
-        <v>1.0362155869924401</v>
+        <v>1.04098612579914</v>
       </c>
       <c r="F4">
-        <v>1.0224624934539399</v>
+        <v>1.0285940071661499</v>
       </c>
       <c r="G4">
-        <v>1.0181875645073499</v>
+        <v>1.0214898311731999</v>
       </c>
       <c r="H4">
-        <v>1.01183180321387</v>
+        <v>1.0163716726575101</v>
       </c>
       <c r="I4">
-        <v>1.0084732947417301</v>
+        <v>1.01228539243496</v>
       </c>
       <c r="J4">
-        <v>1.00868983220162</v>
+        <v>1.0091933506114901</v>
       </c>
       <c r="P4" s="10">
         <v>35430</v>
@@ -3000,16 +2898,16 @@
         <v>120</v>
       </c>
       <c r="R4" s="2">
-        <v>113892219</v>
+        <v>77530054</v>
       </c>
       <c r="S4">
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="T4">
-        <v>1.0082866118107701</v>
+        <v>1.01171918357155</v>
       </c>
       <c r="U4" s="2">
-        <v>114835999.60712001</v>
+        <v>78438642.935137793</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -3017,28 +2915,28 @@
         <v>35795</v>
       </c>
       <c r="B5">
-        <v>1.61364907559491</v>
+        <v>1.56654334176981</v>
       </c>
       <c r="C5">
-        <v>1.1423991351412</v>
+        <v>1.1316236783129601</v>
       </c>
       <c r="D5">
-        <v>1.0556583056618101</v>
+        <v>1.0614681790846301</v>
       </c>
       <c r="E5">
-        <v>1.02564356971795</v>
+        <v>1.03607440892283</v>
       </c>
       <c r="F5">
-        <v>1.01806000140116</v>
+        <v>1.02471111284911</v>
       </c>
       <c r="G5">
-        <v>1.01484881845053</v>
+        <v>1.0174645921701</v>
       </c>
       <c r="H5">
-        <v>1.01184556407597</v>
+        <v>1.0141902334389401</v>
       </c>
       <c r="I5">
-        <v>1.0100279472695399</v>
+        <v>1.0112217910713801</v>
       </c>
       <c r="P5" s="10">
         <v>35795</v>
@@ -3047,16 +2945,16 @@
         <v>108</v>
       </c>
       <c r="R5" s="2">
-        <v>105035099</v>
+        <v>66936974</v>
       </c>
       <c r="S5">
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="T5">
-        <v>1.015503572698</v>
+        <v>1.02009902474493</v>
       </c>
       <c r="U5" s="2">
-        <v>106663518.29318801</v>
+        <v>68282341.896776706</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -3064,25 +2962,25 @@
         <v>36160</v>
       </c>
       <c r="B6">
-        <v>1.6433510835909599</v>
+        <v>1.5889647484479901</v>
       </c>
       <c r="C6">
-        <v>1.1312058899372299</v>
+        <v>1.1494577966492701</v>
       </c>
       <c r="D6">
-        <v>1.05563267121625</v>
+        <v>1.06806476197157</v>
       </c>
       <c r="E6">
-        <v>1.02988201201901</v>
+        <v>1.0420052923385099</v>
       </c>
       <c r="F6">
-        <v>1.02035435584593</v>
+        <v>1.02546370786916</v>
       </c>
       <c r="G6">
-        <v>1.01409958409144</v>
+        <v>1.01668027193238</v>
       </c>
       <c r="H6">
-        <v>1.01138271773294</v>
+        <v>1.01502718826215</v>
       </c>
       <c r="P6" s="10">
         <v>36160</v>
@@ -3091,16 +2989,16 @@
         <v>96</v>
       </c>
       <c r="R6" s="2">
-        <v>111470947</v>
+        <v>71925937</v>
       </c>
       <c r="S6">
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="T6">
-        <v>1.0237143849969601</v>
+        <v>1.0314238650335199</v>
       </c>
       <c r="U6" s="2">
-        <v>114114411.953134</v>
+        <v>74186127.936697498</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -3108,22 +3006,22 @@
         <v>36525</v>
       </c>
       <c r="B7">
-        <v>1.6579937134584499</v>
+        <v>1.5889180550269399</v>
       </c>
       <c r="C7">
-        <v>1.1537179121560599</v>
+        <v>1.14265931799329</v>
       </c>
       <c r="D7">
-        <v>1.0587860154861599</v>
+        <v>1.0651787619228801</v>
       </c>
       <c r="E7">
-        <v>1.0306216931168399</v>
+        <v>1.0386401799064</v>
       </c>
       <c r="F7">
-        <v>1.01878313370386</v>
+        <v>1.0244942107337001</v>
       </c>
       <c r="G7">
-        <v>1.01252453061605</v>
+        <v>1.0185798507005499</v>
       </c>
       <c r="P7" s="10">
         <v>36525</v>
@@ -3132,16 +3030,16 @@
         <v>84</v>
       </c>
       <c r="R7" s="2">
-        <v>115966335</v>
+        <v>67271819</v>
       </c>
       <c r="S7">
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="T7">
-        <v>1.03516629123068</v>
+        <v>1.04614285835599</v>
       </c>
       <c r="U7" s="2">
-        <v>120044440.909565</v>
+        <v>70375933.015466496</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -3149,19 +3047,19 @@
         <v>36891</v>
       </c>
       <c r="B8">
-        <v>1.64952613997375</v>
+        <v>1.59438115261613</v>
       </c>
       <c r="C8">
-        <v>1.1375990783068901</v>
+        <v>1.1365047173371601</v>
       </c>
       <c r="D8">
-        <v>1.0544684265626401</v>
+        <v>1.05800281131913</v>
       </c>
       <c r="E8">
-        <v>1.02880114824938</v>
+        <v>1.0313221627101199</v>
       </c>
       <c r="F8">
-        <v>1.0186547672591599</v>
+        <v>1.02224439978957</v>
       </c>
       <c r="P8" s="10">
         <v>36891</v>
@@ -3170,16 +3068,16 @@
         <v>72</v>
       </c>
       <c r="R8" s="2">
-        <v>113418617</v>
+        <v>66996567</v>
       </c>
       <c r="S8">
-        <v>1.01456179356613</v>
+        <v>1.01778337263625</v>
       </c>
       <c r="T8">
-        <v>1.0502401690701999</v>
+        <v>1.0647468066368799</v>
       </c>
       <c r="U8" s="2">
-        <v>119116787.493789</v>
+        <v>71334380.768883795</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
@@ -3187,16 +3085,16 @@
         <v>37256</v>
       </c>
       <c r="B9">
-        <v>1.6381580598732</v>
+        <v>1.59930776065605</v>
       </c>
       <c r="C9">
-        <v>1.1483746347227499</v>
+        <v>1.14925810923563</v>
       </c>
       <c r="D9">
-        <v>1.0575769747902899</v>
+        <v>1.0690873990763099</v>
       </c>
       <c r="E9">
-        <v>1.0317713151585</v>
+        <v>1.0394574650241499</v>
       </c>
       <c r="P9" s="10">
         <v>37256</v>
@@ -3205,16 +3103,16 @@
         <v>60</v>
       </c>
       <c r="R9" s="2">
-        <v>120298776</v>
+        <v>69639352</v>
       </c>
       <c r="S9">
-        <v>1.01955362337227</v>
+        <v>1.0246273377411199</v>
       </c>
       <c r="T9">
-        <v>1.07077616978663</v>
+        <v>1.0909686858526999</v>
       </c>
       <c r="U9" s="2">
-        <v>128813062.5953</v>
+        <v>75974352.335073903</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -3222,13 +3120,13 @@
         <v>37621</v>
       </c>
       <c r="B10">
-        <v>1.6309711241026399</v>
+        <v>1.6085956329645099</v>
       </c>
       <c r="C10">
-        <v>1.1454358042173001</v>
+        <v>1.1518469266379301</v>
       </c>
       <c r="D10">
-        <v>1.06338854293367</v>
+        <v>1.0712455052685099</v>
       </c>
       <c r="P10" s="10">
         <v>37621</v>
@@ -3237,16 +3135,16 @@
         <v>48</v>
       </c>
       <c r="R10" s="2">
-        <v>111774418</v>
+        <v>69554382</v>
       </c>
       <c r="S10">
-        <v>1.0297559094086799</v>
+        <v>1.03772481931108</v>
       </c>
       <c r="T10">
-        <v>1.1026380884917799</v>
+        <v>1.1321252824005501</v>
       </c>
       <c r="U10" s="2">
-        <v>123246730.605801</v>
+        <v>78744274.363945693</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
@@ -3254,10 +3152,10 @@
         <v>37986</v>
       </c>
       <c r="B11">
-        <v>1.6912595100205301</v>
+        <v>1.6145808481905299</v>
       </c>
       <c r="C11">
-        <v>1.1721053090090801</v>
+        <v>1.13971469647167</v>
       </c>
       <c r="P11" s="10">
         <v>37986</v>
@@ -3266,16 +3164,16 @@
         <v>36</v>
       </c>
       <c r="R11" s="2">
-        <v>130480200</v>
+        <v>66981239</v>
       </c>
       <c r="S11">
-        <v>1.0566080746314901</v>
+        <v>1.0651683677659001</v>
       </c>
       <c r="T11">
-        <v>1.16505630769665</v>
+        <v>1.20590403916111</v>
       </c>
       <c r="U11" s="2">
-        <v>152016780.03952101</v>
+        <v>80772946.658115402</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -3283,7 +3181,7 @@
         <v>38352</v>
       </c>
       <c r="B12">
-        <v>1.61866550511115</v>
+        <v>1.6360532183019201</v>
       </c>
       <c r="P12" s="10">
         <v>38352</v>
@@ -3292,16 +3190,16 @@
         <v>24</v>
       </c>
       <c r="R12" s="2">
-        <v>100442115</v>
+        <v>63274548</v>
       </c>
       <c r="S12">
-        <v>1.1437721330327499</v>
+        <v>1.1426209917621299</v>
       </c>
       <c r="T12">
-        <v>1.3325589381574601</v>
+        <v>1.37789126919623</v>
       </c>
       <c r="U12" s="2">
-        <v>133845038.110689</v>
+        <v>87185447.251537502</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -3315,254 +3213,254 @@
         <v>12</v>
       </c>
       <c r="R13" s="2">
-        <v>68388763</v>
+        <v>40397929</v>
       </c>
       <c r="S13">
-        <v>1.6245863032932999</v>
+        <v>1.5856359313563</v>
       </c>
       <c r="T13">
-        <v>2.1648569992616702</v>
+        <v>2.1848339059396702</v>
       </c>
       <c r="U13" s="2">
-        <v>148051892.25139701</v>
+        <v>88262765.008943394</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="P14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="R14" s="2">
-        <v>1306876488</v>
+        <v>797928173</v>
       </c>
       <c r="U14" s="2">
-        <v>1476812135.2927001</v>
+        <v>911313173.41673601</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15">
-        <v>1.6245863032932999</v>
+        <v>1.5856359313563</v>
       </c>
       <c r="C15">
-        <v>1.1437721330327499</v>
+        <v>1.1426209917621299</v>
       </c>
       <c r="D15">
-        <v>1.0566080746314901</v>
+        <v>1.0651683677659001</v>
       </c>
       <c r="E15">
-        <v>1.0297559094086799</v>
+        <v>1.03772481931108</v>
       </c>
       <c r="F15">
-        <v>1.01955362337227</v>
+        <v>1.0246273377411199</v>
       </c>
       <c r="G15">
-        <v>1.01456179356613</v>
+        <v>1.01778337263625</v>
       </c>
       <c r="H15">
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="I15">
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="J15">
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="K15">
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="L15">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16">
-        <v>1.64767558586787</v>
+        <v>1.6053184840141299</v>
       </c>
       <c r="C16">
-        <v>1.14823438734641</v>
+        <v>1.14315139441475</v>
       </c>
       <c r="D16">
-        <v>1.0581706242215001</v>
+        <v>1.06604837133138</v>
       </c>
       <c r="E16">
-        <v>1.03017718036543</v>
+        <v>1.0380653373381401</v>
       </c>
       <c r="F16">
-        <v>1.01955362337227</v>
+        <v>1.0246273377411199</v>
       </c>
       <c r="G16">
-        <v>1.01456179356613</v>
+        <v>1.01778337263625</v>
       </c>
       <c r="H16">
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="I16">
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="J16">
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="K16">
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="L16">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17">
-        <v>1.6465734975053701</v>
+        <v>1.61136933346213</v>
       </c>
       <c r="C17">
-        <v>1.1522964638259099</v>
+        <v>1.14404641397548</v>
       </c>
       <c r="D17">
-        <v>1.0580122165969199</v>
+        <v>1.0664298291585801</v>
       </c>
       <c r="E17">
-        <v>1.0294570071186</v>
+        <v>1.0375535860260601</v>
       </c>
       <c r="F17">
-        <v>1.0196640545200899</v>
+        <v>1.02516777288521</v>
       </c>
       <c r="G17">
-        <v>1.0146836800132799</v>
+        <v>1.0180391363069601</v>
       </c>
       <c r="H17">
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="I17">
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="J17">
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="K17">
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="L17">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>1.63944020094222</v>
+        <v>1.6076594060239799</v>
       </c>
       <c r="C18">
-        <v>1.14912339719487</v>
+        <v>1.14379607719856</v>
       </c>
       <c r="D18">
-        <v>1.05736513911504</v>
+        <v>1.06749291204261</v>
       </c>
       <c r="E18">
-        <v>1.0297688590055301</v>
+        <v>1.03811099660326</v>
       </c>
       <c r="F18">
-        <v>1.01924658499789</v>
+        <v>1.0249016921215499</v>
       </c>
       <c r="G18">
-        <v>1.0142552467669399</v>
+        <v>1.01755959893682</v>
       </c>
       <c r="H18">
-        <v>1.0113001982655501</v>
+        <v>1.0141847833220901</v>
       </c>
       <c r="I18">
-        <v>1.0080264044413501</v>
+        <v>1.01123200334186</v>
       </c>
       <c r="J18">
-        <v>1.00727726461376</v>
+        <v>1.0080729015504599</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19">
-        <v>1.6483747738296199</v>
+        <v>1.62021766324591</v>
       </c>
       <c r="C19">
-        <v>1.15630552743565</v>
+        <v>1.1468125006206999</v>
       </c>
       <c r="D19">
-        <v>1.05849466746299</v>
+        <v>1.0662862278365799</v>
       </c>
       <c r="E19">
-        <v>1.0304330487339399</v>
+        <v>1.0365100248800301</v>
       </c>
       <c r="F19">
-        <v>1.01924658499789</v>
+        <v>1.0240822583893301</v>
       </c>
       <c r="G19">
-        <v>1.01377748160973</v>
+        <v>1.01755959893682</v>
       </c>
       <c r="H19">
-        <v>1.0116832379532299</v>
+        <v>1.0152442913646</v>
       </c>
       <c r="I19">
-        <v>1.0086766558373099</v>
+        <v>1.0116188837822999</v>
       </c>
       <c r="J19">
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="K19">
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="L19">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21">
-        <v>1.6245863032932999</v>
+        <v>1.5856359313563</v>
       </c>
       <c r="C21">
-        <v>1.1437721330327499</v>
+        <v>1.1426209917621299</v>
       </c>
       <c r="D21">
-        <v>1.0566080746314901</v>
+        <v>1.0651683677659001</v>
       </c>
       <c r="E21">
-        <v>1.0297559094086799</v>
+        <v>1.03772481931108</v>
       </c>
       <c r="F21">
-        <v>1.01955362337227</v>
+        <v>1.0246273377411199</v>
       </c>
       <c r="G21">
-        <v>1.01456179356613</v>
+        <v>1.01778337263625</v>
       </c>
       <c r="H21">
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="I21">
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="J21">
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="K21">
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="L21">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -3570,40 +3468,40 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24">
-        <v>1.6245863032932999</v>
+        <v>1.5856359313563</v>
       </c>
       <c r="C24">
-        <v>1.1437721330327499</v>
+        <v>1.1426209917621299</v>
       </c>
       <c r="D24">
-        <v>1.0566080746314901</v>
+        <v>1.0651683677659001</v>
       </c>
       <c r="E24">
-        <v>1.0297559094086799</v>
+        <v>1.03772481931108</v>
       </c>
       <c r="F24">
-        <v>1.01955362337227</v>
+        <v>1.0246273377411199</v>
       </c>
       <c r="G24">
-        <v>1.01456179356613</v>
+        <v>1.01778337263625</v>
       </c>
       <c r="H24">
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="I24">
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="J24">
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="K24">
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="L24">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -3611,40 +3509,40 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25">
-        <v>2.1648569992616702</v>
+        <v>2.1848339059396702</v>
       </c>
       <c r="C25">
-        <v>1.3325589381574601</v>
+        <v>1.37789126919623</v>
       </c>
       <c r="D25">
-        <v>1.16505630769665</v>
+        <v>1.20590403916111</v>
       </c>
       <c r="E25">
-        <v>1.1026380884917799</v>
+        <v>1.1321252824005501</v>
       </c>
       <c r="F25">
-        <v>1.07077616978663</v>
+        <v>1.0909686858526999</v>
       </c>
       <c r="G25">
-        <v>1.0502401690701999</v>
+        <v>1.0647468066368799</v>
       </c>
       <c r="H25">
-        <v>1.03516629123068</v>
+        <v>1.04614285835599</v>
       </c>
       <c r="I25">
-        <v>1.0237143849969601</v>
+        <v>1.0314238650335199</v>
       </c>
       <c r="J25">
-        <v>1.015503572698</v>
+        <v>1.02009902474493</v>
       </c>
       <c r="K25">
-        <v>1.0082866118107701</v>
+        <v>1.01171918357155</v>
       </c>
       <c r="L25">
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -3655,37 +3553,37 @@
         <v>5</v>
       </c>
       <c r="B26">
-        <v>0.46192427506345801</v>
+        <v>0.457700696277831</v>
       </c>
       <c r="C26">
-        <v>0.75043585042678196</v>
+        <v>0.72574666982492497</v>
       </c>
       <c r="D26">
-        <v>0.85832761334688401</v>
+        <v>0.82925337964342205</v>
       </c>
       <c r="E26">
-        <v>0.90691588694149805</v>
+        <v>0.88329446885914198</v>
       </c>
       <c r="F26">
-        <v>0.93390199391462403</v>
+        <v>0.91661659309533405</v>
       </c>
       <c r="G26">
-        <v>0.95216316177024496</v>
+        <v>0.93919041951260696</v>
       </c>
       <c r="H26">
-        <v>0.966028365173217</v>
+        <v>0.95589239271919502</v>
       </c>
       <c r="I26">
-        <v>0.97683495968747902</v>
+        <v>0.96953350984127296</v>
       </c>
       <c r="J26">
-        <v>0.98473311850906498</v>
+        <v>0.98029698660876996</v>
       </c>
       <c r="K26">
-        <v>0.99178149177654296</v>
+        <v>0.98841656483158302</v>
       </c>
       <c r="L26">
-        <v>0.99667690044138102</v>
+        <v>0.99494757802231004</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -3738,7 +3636,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" s="13">
         <f ca="1">+OFFSET($B$35,B28,0)</f>
@@ -3787,146 +3685,146 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" s="13">
         <f t="shared" ref="B30:I30" si="2">+B15</f>
-        <v>1.6245863032932999</v>
+        <v>1.5856359313563</v>
       </c>
       <c r="C30" s="13">
         <f t="shared" si="2"/>
-        <v>1.1437721330327499</v>
+        <v>1.1426209917621299</v>
       </c>
       <c r="D30" s="13">
         <f t="shared" si="2"/>
-        <v>1.0566080746314901</v>
+        <v>1.0651683677659001</v>
       </c>
       <c r="E30" s="13">
         <f t="shared" si="2"/>
-        <v>1.0297559094086799</v>
+        <v>1.03772481931108</v>
       </c>
       <c r="F30" s="13">
         <f t="shared" si="2"/>
-        <v>1.01955362337227</v>
+        <v>1.0246273377411199</v>
       </c>
       <c r="G30" s="13">
         <f t="shared" si="2"/>
-        <v>1.01456179356613</v>
+        <v>1.01778337263625</v>
       </c>
       <c r="H30" s="13">
         <f t="shared" si="2"/>
-        <v>1.0111866223641599</v>
+        <v>1.0142705572572599</v>
       </c>
       <c r="I30" s="13">
         <f t="shared" si="2"/>
-        <v>1.00808545880065</v>
+        <v>1.01110170680873</v>
       </c>
       <c r="J30" s="13">
         <f>+J15</f>
-        <v>1.0071576482348299</v>
+        <v>1.0082827738264299</v>
       </c>
       <c r="K30" s="13">
         <f t="shared" ref="K30:L30" si="3">+K15</f>
-        <v>1.0049359750161</v>
+        <v>1.00660755133322</v>
       </c>
       <c r="L30" s="13">
         <f t="shared" si="3"/>
-        <v>1.0033341793686099</v>
+        <v>1.0050780785734801</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B31" s="14">
         <f ca="1">+B29-B15</f>
-        <v>0</v>
+        <v>3.8950371936999906E-2</v>
       </c>
       <c r="C31" s="14">
         <f ca="1">+C29-C15</f>
-        <v>-9.9920072216264089E-15</v>
+        <v>1.151141270610001E-3</v>
       </c>
       <c r="D31" s="14">
         <f ca="1">+D29-D15</f>
-        <v>0</v>
+        <v>-8.5602931344099797E-3</v>
       </c>
       <c r="E31" s="14">
         <f t="shared" ref="E31:L31" ca="1" si="4">+E29-E15</f>
-        <v>0</v>
+        <v>-7.9689099024000676E-3</v>
       </c>
       <c r="F31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>-5.0737143688499575E-3</v>
       </c>
       <c r="G31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>-3.2215790701199953E-3</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>-3.0839348930999932E-3</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-9.9920072216264089E-15</v>
+        <v>-3.0162480080899723E-3</v>
       </c>
       <c r="J31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>-1.1251255916000513E-3</v>
       </c>
       <c r="K31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-9.9920072216264089E-15</v>
+        <v>-1.6715763171299969E-3</v>
       </c>
       <c r="L31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-9.9920072216264089E-15</v>
+        <v>-1.7438992048801616E-3</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33">
         <f>1/B24</f>
-        <v>0.61554132148771523</v>
+        <v>0.63066179330625627</v>
       </c>
       <c r="C33">
         <f t="shared" ref="C33:M33" si="5">1/C24</f>
-        <v>0.87430002106142124</v>
+        <v>0.87518084054960132</v>
       </c>
       <c r="D33">
         <f t="shared" si="5"/>
-        <v>0.94642471888052426</v>
+        <v>0.93881871661042171</v>
       </c>
       <c r="E33">
         <f t="shared" si="5"/>
-        <v>0.97110391973786614</v>
+        <v>0.96364660591222584</v>
       </c>
       <c r="F33">
         <f t="shared" si="5"/>
-        <v>0.98082138798389584</v>
+        <v>0.97596459040863281</v>
       </c>
       <c r="G33">
         <f t="shared" si="5"/>
-        <v>0.9856472088161865</v>
+        <v>0.98252735000947433</v>
       </c>
       <c r="H33">
         <f t="shared" si="5"/>
-        <v>0.98893713374292325</v>
+        <v>0.98593022625457094</v>
       </c>
       <c r="I33">
         <f t="shared" si="5"/>
-        <v>0.99197939149894143</v>
+        <v>0.98902018784661183</v>
       </c>
       <c r="J33">
         <f t="shared" si="5"/>
-        <v>0.99289321959936006</v>
+        <v>0.99178526694947211</v>
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>0.99508826916458937</v>
+        <v>0.99343582181112344</v>
       </c>
       <c r="L33">
         <f t="shared" si="5"/>
-        <v>0.99667690044137824</v>
+        <v>0.99494757802230904</v>
       </c>
       <c r="M33">
         <f t="shared" si="5"/>
@@ -3935,7 +3833,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
@@ -4047,7 +3945,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="N5" sqref="N5:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4066,33 +3964,33 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
         <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
       </c>
       <c r="H2" t="str">
         <f>+E2</f>
@@ -4161,486 +4059,318 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>402632</v>
+        <v>276189</v>
       </c>
       <c r="B4" s="2">
-        <v>354474</v>
+        <v>336589</v>
       </c>
       <c r="C4" s="2">
-        <v>156682</v>
+        <v>84740</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ref="E4:E15" si="0">+B4</f>
-        <v>354474</v>
+        <v>336589</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F15" si="1">+E4-$A4</f>
-        <v>-48158</v>
+        <v>60400</v>
       </c>
       <c r="H4" s="2">
         <v>397347.757547274</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ref="I4:I15" si="2">+H4-$A4</f>
-        <v>-5284.2424527260009</v>
+        <v>121158.757547274</v>
       </c>
       <c r="K4" s="2">
         <v>395498.34646560898</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ref="L4:L15" si="3">+K4-$A4</f>
-        <v>-7133.6535343910218</v>
+        <v>119309.34646560898</v>
       </c>
       <c r="N4" s="2">
         <v>392983.70867947099</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" ref="O4:O15" si="4">+N4-$A4</f>
-        <v>-9648.2913205290097</v>
+        <v>116794.70867947099</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>1362840</v>
+        <v>822196</v>
       </c>
       <c r="B5" s="2">
-        <v>943781</v>
+        <v>908589</v>
       </c>
       <c r="C5" s="2">
-        <v>244760</v>
+        <v>129090</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>943781</v>
+        <v>908589</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>-419059</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1042026.98218798</v>
-      </c>
-      <c r="I5" s="2">
-        <f t="shared" si="2"/>
-        <v>-320813.01781202003</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1035041.96517976</v>
-      </c>
-      <c r="L5" s="2">
-        <f t="shared" si="3"/>
-        <v>-327798.03482023999</v>
-      </c>
-      <c r="N5" s="2">
-        <v>1035549.28526323</v>
-      </c>
-      <c r="O5" s="2">
-        <f t="shared" si="4"/>
-        <v>-327290.71473677002</v>
-      </c>
+        <v>86393</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>2052225</v>
+        <v>1484528</v>
       </c>
       <c r="B6" s="2">
-        <v>1628419</v>
+        <v>1345368</v>
       </c>
       <c r="C6" s="2">
-        <v>308702</v>
+        <v>136753</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>1628419</v>
+        <v>1345368</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>-423806</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1632331.0212202601</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="2"/>
-        <v>-419893.97877973993</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1625718.6803675201</v>
-      </c>
-      <c r="L6" s="2">
-        <f t="shared" si="3"/>
-        <v>-426506.31963247992</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1634315.77447871</v>
-      </c>
-      <c r="O6" s="2">
-        <f t="shared" si="4"/>
-        <v>-417909.22552128998</v>
-      </c>
+        <v>-139160</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>2932050</v>
+        <v>1991356</v>
       </c>
       <c r="B7" s="2">
-        <v>2643465</v>
+        <v>2260191</v>
       </c>
       <c r="C7" s="2">
-        <v>376423</v>
+        <v>171977</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>2643465</v>
+        <v>2260191</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>-288585</v>
-      </c>
-      <c r="H7" s="2">
-        <v>2829130.2551132301</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="2"/>
-        <v>-102919.74488676991</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2806639.6286765202</v>
-      </c>
-      <c r="L7" s="2">
-        <f t="shared" si="3"/>
-        <v>-125410.37132347981</v>
-      </c>
-      <c r="N7" s="2">
-        <v>2792521.1611041599</v>
-      </c>
-      <c r="O7" s="2">
-        <f t="shared" si="4"/>
-        <v>-139528.8388958401</v>
-      </c>
+        <v>268835</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>3760055</v>
+        <v>2893142</v>
       </c>
       <c r="B8" s="2">
-        <v>4078106</v>
+        <v>3104114</v>
       </c>
       <c r="C8" s="2">
-        <v>399908</v>
+        <v>208287</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>4078106</v>
+        <v>3104114</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>318051</v>
-      </c>
-      <c r="H8" s="2">
-        <v>4261071.6386745097</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="2"/>
-        <v>501016.63867450971</v>
-      </c>
-      <c r="K8" s="2">
-        <v>4229964.9832931198</v>
-      </c>
-      <c r="L8" s="2">
-        <f t="shared" si="3"/>
-        <v>469909.98329311982</v>
-      </c>
-      <c r="N8" s="2">
-        <v>4303230.8501152704</v>
-      </c>
-      <c r="O8" s="2">
-        <f t="shared" si="4"/>
-        <v>543175.85011527035</v>
-      </c>
+        <v>210972</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>5584206</v>
+        <v>3652487</v>
       </c>
       <c r="B9" s="2">
-        <v>5698170</v>
+        <v>4337814</v>
       </c>
       <c r="C9" s="2">
-        <v>465201</v>
+        <v>266134</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>5698170</v>
+        <v>4337814</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>113964</v>
-      </c>
-      <c r="H9" s="2">
-        <v>5854183.32412122</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="2"/>
-        <v>269977.32412122004</v>
-      </c>
-      <c r="K9" s="2">
-        <v>5925973.0781548005</v>
-      </c>
-      <c r="L9" s="2">
-        <f t="shared" si="3"/>
-        <v>341767.07815480046</v>
-      </c>
-      <c r="N9" s="2">
-        <v>5890531.7190064499</v>
-      </c>
-      <c r="O9" s="2">
-        <f t="shared" si="4"/>
-        <v>306325.71900644992</v>
-      </c>
+        <v>685327</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>7233582</v>
+        <v>5656252</v>
       </c>
       <c r="B10" s="2">
-        <v>8514287</v>
+        <v>6335000</v>
       </c>
       <c r="C10" s="2">
-        <v>525346</v>
+        <v>323050</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>8514287</v>
+        <v>6335000</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>1280705</v>
-      </c>
-      <c r="H10" s="2">
-        <v>9033022.3294650093</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="2"/>
-        <v>1799440.3294650093</v>
-      </c>
-      <c r="K10" s="2">
-        <v>9019704.0498889796</v>
-      </c>
-      <c r="L10" s="2">
-        <f t="shared" si="3"/>
-        <v>1786122.0498889796</v>
-      </c>
-      <c r="N10" s="2">
-        <v>8884233.9282880891</v>
-      </c>
-      <c r="O10" s="2">
-        <f t="shared" si="4"/>
-        <v>1650651.9282880891</v>
-      </c>
+        <v>678748</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>12818962</v>
+        <v>8988414</v>
       </c>
       <c r="B11" s="2">
-        <v>11472313</v>
+        <v>9189892</v>
       </c>
       <c r="C11" s="2">
-        <v>652233</v>
+        <v>424715</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>11472313</v>
+        <v>9189892</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>-1346649</v>
-      </c>
-      <c r="H11" s="2">
-        <v>11607119.2664591</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="2"/>
-        <v>-1211842.7335409001</v>
-      </c>
-      <c r="K11" s="2">
-        <v>11613937.612503899</v>
-      </c>
-      <c r="L11" s="2">
-        <f t="shared" si="3"/>
-        <v>-1205024.3874961007</v>
-      </c>
-      <c r="N11" s="2">
-        <v>11709940.6135024</v>
-      </c>
-      <c r="O11" s="2">
-        <f t="shared" si="4"/>
-        <v>-1109021.3864976</v>
-      </c>
+        <v>201478</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>24357870</v>
+        <v>11357731</v>
       </c>
       <c r="B12" s="2">
-        <v>21536580</v>
+        <v>13791708</v>
       </c>
       <c r="C12" s="2">
-        <v>943736</v>
+        <v>550837</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>21536580</v>
+        <v>13791708</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>-2821290</v>
-      </c>
-      <c r="H12" s="2">
-        <v>22326013.2191143</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="2"/>
-        <v>-2031856.7808857001</v>
-      </c>
-      <c r="K12" s="2">
-        <v>22217740.400923599</v>
-      </c>
-      <c r="L12" s="2">
-        <f t="shared" si="3"/>
-        <v>-2140129.5990764014</v>
-      </c>
-      <c r="N12" s="2">
-        <v>22172499.960506499</v>
-      </c>
-      <c r="O12" s="2">
-        <f t="shared" si="4"/>
-        <v>-2185370.0394935012</v>
-      </c>
+        <v>2433977</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>31901613</v>
+        <v>24707983</v>
       </c>
       <c r="B13" s="2">
-        <v>33402923</v>
+        <v>23910899</v>
       </c>
       <c r="C13" s="2">
-        <v>2055725</v>
+        <v>871506</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>33402923</v>
+        <v>23910899</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="1"/>
-        <v>1501310</v>
-      </c>
-      <c r="H13" s="2">
-        <v>32942178.184202898</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="2"/>
-        <v>1040565.1842028983</v>
-      </c>
-      <c r="K13" s="2">
-        <v>33069630.074163701</v>
-      </c>
-      <c r="L13" s="2">
-        <f t="shared" si="3"/>
-        <v>1168017.0741637014</v>
-      </c>
-      <c r="N13" s="2">
-        <v>33196141.2637177</v>
-      </c>
-      <c r="O13" s="2">
-        <f t="shared" si="4"/>
-        <v>1294528.2637176998</v>
-      </c>
+        <v>-797084</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>77968325</v>
+        <v>46512588</v>
       </c>
       <c r="B14" s="2">
-        <v>79663129</v>
+        <v>47864836</v>
       </c>
       <c r="C14" s="2">
-        <v>4164702</v>
+        <v>2120540</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>79663129</v>
+        <v>47864836</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="1"/>
-        <v>1694804</v>
-      </c>
-      <c r="H14" s="2">
-        <v>80190188.241816998</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="2"/>
-        <v>2221863.2418169975</v>
-      </c>
-      <c r="K14" s="2">
-        <v>80891595.4263978</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="3"/>
-        <v>2923270.4263978004</v>
-      </c>
-      <c r="N14" s="2">
-        <v>81701168.405678198</v>
-      </c>
-      <c r="O14" s="2">
-        <f t="shared" si="4"/>
-        <v>3732843.4056781977</v>
-      </c>
+        <v>1352248</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>170374360</v>
+        <v>108342866</v>
       </c>
       <c r="B15" s="2">
-        <v>169935647</v>
+        <v>113385000</v>
       </c>
       <c r="C15" s="2">
-        <v>5505571</v>
+        <v>2766715</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>169935647</v>
+        <v>113385000</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>-438713</v>
-      </c>
-      <c r="H15" s="2">
-        <f>+SUM(H3:H14)</f>
-        <v>172114612.21992278</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="2"/>
-        <v>1740252.219922781</v>
-      </c>
-      <c r="K15" s="2">
-        <f>+SUM(K3:K14)</f>
-        <v>172831444.24601531</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="3"/>
-        <v>2457084.2460153103</v>
-      </c>
-      <c r="N15" s="2">
-        <f>+SUM(N3:N14)</f>
-        <v>173713116.67034018</v>
-      </c>
-      <c r="O15" s="2">
-        <f t="shared" si="4"/>
-        <v>3338756.6703401804</v>
-      </c>
+        <v>5042134</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor update to tutorial
</commit_message>
<xml_diff>
--- a/data/reservingAccident/triangle.xlsx
+++ b/data/reservingAccident/triangle.xlsx
@@ -1106,7 +1106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C3">
         <v>1</v>
       </c>
@@ -2682,7 +2682,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M26"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3593,23 +3593,23 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C28">
-        <f>1+B28</f>
-        <v>2</v>
+        <f>+B28-1</f>
+        <v>10</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:L28" si="0">1+C28</f>
-        <v>3</v>
+        <f t="shared" ref="D28:L28" si="0">+C28-1</f>
+        <v>9</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -3617,23 +3617,23 @@
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L28">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
@@ -3642,47 +3642,47 @@
       </c>
       <c r="B29" s="13">
         <f ca="1">+OFFSET($B$35,B28,0)</f>
-        <v>1.6245863032932999</v>
+        <v>1.5929067447573599</v>
       </c>
       <c r="C29" s="13">
         <f t="shared" ref="C29:L29" ca="1" si="1">+OFFSET($B$35,C28,0)</f>
-        <v>1.1437721330327399</v>
+        <v>1.1403086228617001</v>
       </c>
       <c r="D29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0566080746314901</v>
+        <v>1.06243631905238</v>
       </c>
       <c r="E29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0297559094086799</v>
+        <v>1.0355982667967401</v>
       </c>
       <c r="F29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.01955362337227</v>
+        <v>1.0233931849600699</v>
       </c>
       <c r="G29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.01456179356613</v>
+        <v>1.01691014686438</v>
       </c>
       <c r="H29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0111866223641599</v>
+        <v>1.0128410248044</v>
       </c>
       <c r="I29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.00808545880064</v>
+        <v>1.0098787501966899</v>
       </c>
       <c r="J29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0071576482348299</v>
+        <v>1.00853969396661</v>
       </c>
       <c r="K29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.00493597501609</v>
+        <v>1.00672672595653</v>
       </c>
       <c r="L29" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0033341793685999</v>
+        <v>1.00423324917742</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -3737,47 +3737,47 @@
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B31" s="14">
         <f ca="1">+B29-B15</f>
-        <v>3.1679558535939956E-2</v>
+        <v>0</v>
       </c>
       <c r="C31" s="14">
         <f ca="1">+C29-C15</f>
-        <v>3.4635101710398519E-3</v>
+        <v>0</v>
       </c>
       <c r="D31" s="14">
         <f ca="1">+D29-D15</f>
-        <v>-5.8282444208999085E-3</v>
+        <v>-9.9920072216264089E-15</v>
       </c>
       <c r="E31" s="14">
         <f t="shared" ref="E31:L31" ca="1" si="4">+E29-E15</f>
-        <v>-5.8423573880601598E-3</v>
+        <v>0</v>
       </c>
       <c r="F31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-3.8395615878099587E-3</v>
+        <v>-9.9920072216264089E-15</v>
       </c>
       <c r="G31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.3483532982599975E-3</v>
+        <v>-9.9920072216264089E-15</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.6544024402400659E-3</v>
+        <v>0</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.7932913960498897E-3</v>
+        <v>0</v>
       </c>
       <c r="J31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.3820457317801349E-3</v>
+        <v>0</v>
       </c>
       <c r="K31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.7907509404400113E-3</v>
+        <v>0</v>
       </c>
       <c r="L31" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>-8.9906980883003307E-4</v>
+        <v>-9.9920072216264089E-15</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -3843,7 +3843,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="12">
-        <v>1.6245863032932999</v>
+        <v>1.00423324917742</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
@@ -3852,7 +3852,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="12">
-        <v>1.1437721330327399</v>
+        <v>1.00672672595653</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
@@ -3861,7 +3861,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="12">
-        <v>1.0566080746314901</v>
+        <v>1.00853969396661</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
@@ -3870,7 +3870,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="12">
-        <v>1.0297559094086799</v>
+        <v>1.0098787501966899</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
@@ -3879,7 +3879,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="12">
-        <v>1.01955362337227</v>
+        <v>1.0128410248044</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
@@ -3888,7 +3888,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="12">
-        <v>1.01456179356613</v>
+        <v>1.01691014686438</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
@@ -3897,7 +3897,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="12">
-        <v>1.0111866223641599</v>
+        <v>1.0233931849600699</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
@@ -3906,7 +3906,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="12">
-        <v>1.00808545880064</v>
+        <v>1.0355982667967401</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
@@ -3915,7 +3915,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="12">
-        <v>1.0071576482348299</v>
+        <v>1.06243631905238</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
@@ -3924,7 +3924,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="12">
-        <v>1.00493597501609</v>
+        <v>1.1403086228617001</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
@@ -3933,7 +3933,7 @@
         <v>11</v>
       </c>
       <c r="B46" s="12">
-        <v>1.0033341793685999</v>
+        <v>1.5929067447573599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>